<commit_message>
feat: fix Docker setup and update README
- Use host port 5433 for DB to avoid conflict with local Postgres
- Add /live endpoint and defensive health check
- Document host-based ingest when "db" hostname fails
- Update README with full command flow (pip3/python3)
- Add troubleshooting for port conflicts and empty API response
</commit_message>
<xml_diff>
--- a/eval_results.xlsx
+++ b/eval_results.xlsx
@@ -471,13 +471,21 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Based on the context provided, Alphabet's main risks include:
-1. Cybersecurity threats and incidents, including material breaches of security, data exfiltration or compromise by nation-states and state-sponsored actors, and retaliation attacks (Sections 3-5).
-2. Intellectual property rights infringement, including unauthorized use of trademarks, copyrights, and patents, which could harm business and ability to compete (Section 6).
-3. Geopolitical tensions and armed conflicts that may increase the risk of cyber attacks and data exfiltration or compromise by nation-states and state-sponsored actors.
-4. System errors, vulnerabilities in systems, employee or insider error or malfeasance, which could result in significant legal, financial, and reputational harm (Section 3).
-5. Loss of competitive advantage due to compromised trade secrets and other sensitive information.
-These risks are not explicitly listed as separate items, but they are mentioned throughout the context as potential threats to Alphabet's business and operations.</t>
+          <t>According to the provided text, Alphabet's main risks include:
+1. Cybersecurity threats and data breaches, which could compromise their systems, intellectual property, and customer data ([2], [5])
+2. Materiality analysis and disclosure matters related to cybersecurity incidents ([1], [5])
+3. Theft of intellectual property and attempts to compromise their infrastructure ([5])
+4. Retaliatory attacks in response to security incidents ([2])
+5. Geopolitical tensions or armed conflicts that could increase the risk of cyber attacks ([2])
+6. Insider errors, system errors, or vulnerabilities in their systems that could lead to significant legal, financial, and reputational harm ([3], [5])
+7. Loss of intellectual property rights due to unauthorized use or disclosure, which could harm their business and ability to compete ([4], [5])
+These risks are managed through Alphabet's comprehensive cybersecurity risk management system and processes, including incident management teams, a cross-functional working group, and external experts and internal threat intelligence teams ([5]).
+References:
+[1] (GOOGL)
+[2] (GOOGL)
+[3] (GOOGL)
+[4] (GOOGL)
+[5] (GOOGL)</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -489,7 +497,7 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>12.67</v>
+        <v>19.62</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -511,18 +519,13 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Alphabet faces various cybersecurity threats, including:
-1. Cyber attacks and attempts to gain unauthorized access to their systems on a regular basis ([1], [2])
-2. Development and implementation of AI technologies that may further increase their exposure to or exacerbate the risks of cyber attacks or other security incidents ([1], [2])
-3. Industry-wide software supply chain vulnerabilities and attacks on telecommunications ([1], [2])
-4. Theft of intellectual property and attempts to compromise their infrastructure ([3], [4], [5])
-These threats are addressed through Alphabet's comprehensive cybersecurity risk management process, which includes identifying, assessing, and managing material risks from cybersecurity threats, as well as incident management, remediation, and compliance with disclosure requirements.
-References:
-[1] Alphabet Inc. (2022). 2022 Form 10-K. Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1018724/0001197030216-111351/dt022k.htm#securities-and-exchange-commission&gt;
-[2] Alphabet Inc. (2022). 2022 Proxy Statement (Definitive). Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1018724/0001197030216-113144/dt021p.htm#executive-compensation&gt;
-[3] Alphabet Inc. (2022). 2022 Form 10-K. Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1018724/0001197030216-111351/dt022k.htm#material-risk-management&gt;
-[4] Alphabet Inc. (2022). 2022 Proxy Statement (Definitive). Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1018724/0001197030216-113144/dt021p.htm#material-risks&gt;
-[5] Alphabet Inc. (2022). 2022 Form 10-K. Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1018724/0001197030216-111351/dt022k.htm#executive-compensation&gt;</t>
+          <t>Based on the provided context, Alphabet faces various cybersecurity threats, including:
+1. Bugs, theft, misuse, and security vulnerabilities or breaches ([1])
+2. Cyber attacks and attempts to gain unauthorized access to systems ([1] and [2])
+3. Exploitation of AI technologies by third parties to breach systems ([2])
+4. Industry-wide software supply chain vulnerabilities and attacks on telecommunications ([1])
+5. Attempts to compromise infrastructure, intellectual property theft, and vulnerability in products and services ([2], [4], and [5])
+These threats are managed through Alphabet's comprehensive risk management system and processes, which include incident management teams, dedicated privacy, safety, and security professionals, and a Risk and Compliance Committee that oversees cybersecurity risks.</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -534,7 +537,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>17.47</v>
+        <v>9.59</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -556,10 +559,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Alphabet maintains a comprehensive process for identifying, assessing, and managing material cybersecurity threats as part of its broader risk management system and processes. This includes obtaining input from external experts and internal threat intelligence teams, overseeing cybersecurity risk management and mitigation by dedicated privacy, safety, and security professionals, and having an executive leadership team that regularly considers cybersecurity risks in the context of other material risks to the company.
-According to [1], Alphabet's incident management teams track and log privacy and security incidents across Alphabet, its vendors, and other third-party service providers, remediate and resolve any such incidents, and review significant incidents by a cross-functional working group to determine whether further escalation is appropriate. Any incident assessed as potentially being or potentially becoming material is promptly escalated for further assessment, and then reported to designated members of senior management.
-Alphabet also consults with outside counsel as appropriate, including on materiality analysis and disclosure matters, and its senior management makes the final materiality determinations and disclosure and other compliance decisions. The company's management apprises Alphabet's independent public accounting firm of relevant matters and developments.
-In summary, Alphabet manages cybersecurity risks through a comprehensive process that includes identifying, assessing, and mitigating threats, as well as tracking and responding to incidents, consulting with outside counsel, and regularly reviewing and reporting on materiality determinations and compliance decisions.</t>
+          <t>Alphabet maintains a comprehensive process for identifying, assessing, and managing material risks from cybersecurity threats as part of its broader risk management system and processes. The company obtains input on the security industry and threat trends from multiple external experts and internal threat intelligence teams. Teams of dedicated privacy, safety, and security professionals oversee cybersecurity risk management and mitigation, incident prevention, detection, and remediation.
+The executive leadership team, along with input from these teams, is responsible for the overall enterprise risk management system and processes and regularly considers cybersecurity risks in the context of other material risks to the company. [1]
+In addition, Alphabet's Risk and Compliance Committee has oversight responsibility for risks and incidents relating to cybersecurity threats, including compliance with disclosure requirements, cooperation with law enforcement, and related effects on financial and other risks. The committee reports any findings and recommendations as appropriate to the full Board for consideration.
+Internal Audit maintains a dedicated cybersecurity auditing team that independently tests the company's cybersecurity controls. [5]
+Overall, Alphabet's approach to managing cybersecurity risks involves a multi-layered process that includes input from external experts, internal teams, and the executive leadership team, as well as ongoing monitoring and testing by Internal Audit.</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -571,7 +575,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>12.97</v>
+        <v>11.68</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -593,14 +597,13 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Alphabet's revenue sources or business segments include:
-1. Revenues from Other Bets, which are primarily generated from the sale of autonomous transportation services and internet services [1].
-2. Certain reportable segments that meet specific quantitative thresholds, including:
-* Revenue: 10% or more of the combined revenue, internal and external, of all operating segments (e.g., sales to external customers and intersegment sales or transfers) [5]
-* Profit/Loss: 10% or more of the greater absolute amount of combined reported profit or loss of all operating segments that did not report a loss or combined reported loss of all operating segments that did report a loss [5]
-* Assets: 10% or more of the combined assets of all operating segments [5]
-Additionally, Alphabet's revenue sources may also include subscription-based products, apps, and in-app purchases, as well as devices (as mentioned in [3] and [4]).
-It is worth noting that certain costs associated with Alphabet-level activities, such as AI-focused shared research and development activities, are not allocated to operating segments because they represent Alphabet-level activities [2].</t>
+          <t>Alphabet's revenue sources can be categorized into several business segments:
+1. Google Services segment: This includes revenues from online advertising, including sales to external customers and intersegment sales or transfers that exceed 10% of the combined revenue of all operating segments.
+2. Google Cloud segment: This includes revenues from cloud-based solutions that provide enterprise customers with infrastructure, platform services, and applications.
+3. Other Bets segment: This segment generates revenues primarily from autonomous transportation services and internet services.
+Additionally, Alphabet reports certain costs as Alphabet-level activities, which include:
+* AI-focused shared research and development activities, including employee compensation expenses and technical infrastructure usage costs associated with the development of general AI models.
+These business segments are reported in detail in Alphabet's annual report, including information on revenue recognition, monetization metrics, and fluctuations in revenues due to various factors such as changes in foreign currency exchange rates.</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -612,21 +615,17 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>12.5</v>
+        <v>10.55</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>revenue</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>advertising, cloud</t>
-        </is>
-      </c>
+          <t>revenue, advertising, cloud</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -638,11 +637,10 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Unfortunately, the text snippet you provided doesn't explicitly mention content licensing commitments. However, it does touch on some related topics:
-* Copyright and other intellectual property laws, including the EU Directive on Copyright in the Digital Single Market, which introduce new licensing regimes (References [5] and [6]).
-* Liability with respect to content uploaded by users or linked to from Alphabet's platforms (Reference [5]).
-* The scope of the text and data mining exception being challenged before courts in the EU, which could harm some aspects of Alphabet's business (References [5] and [6]).
-Given this context, it appears that Alphabet is dealing with various copyright-related issues, but the text doesn't explicitly state any content licensing commitments.</t>
+          <t>Alphabet has committed to respecting copyright and other intellectual property rights, including those of users and news publications. According to [3], Alphabet is responsible for creating property rights in news publications that could require payments to news agencies and publishers, which may result in other regulatory actions.
+Additionally, Alphabet has licensing commitments related to its content distribution practices. For example, it has agreed to make changes to its Android agreements as a result of investigations by the Australian Competition and Consumer Commission (ACCC) [4] and the Japanese Fair Trade Commission (JFTC) [6]. These agreements require Alphabet to ensure that its distribution practices are consistent with antitrust law in these countries.
+Alphabet has also committed to respecting the terms of its power purchase agreements, which do not include a minimum dollar commitment [5].
+It's worth noting that Alphabet's content licensing commitments are subject to ongoing evaluation and revision, as the company seeks to comply with changing regulatory requirements and intellectual property laws.</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -654,7 +652,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>10.91</v>
+        <v>11.07</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -680,10 +678,9 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>According to the provided context, Teams of dedicated privacy, safety, and security professionals oversee cybersecurity risk management and mitigation, incident prevention, detection, and remediation. These teams comprise professionals with deep cybersecurity expertise across multiple industries and are led by our Vice President of Privacy, Safety, and Security, who has more than 20 years of experience.
-Additionally, Internal Audit maintains a dedicated cybersecurity auditing team that independently tests our cybersecurity controls (as mentioned in [3] and [4]).
-Senior management regularly discusses cybersecurity risks and trends with the Risk and Compliance Committee, which is overseen by our executive leadership team. Our senior management makes the final materiality determinations and disclosure decisions for cybersecurity-related matters.
-It's worth noting that Alphabet's Vice President of Privacy, Safety, and Security leads the teams overseeing cybersecurity risk management and mitigation, indicating a clear line of oversight and responsibility within the organization.</t>
+          <t>According to the provided context, teams of dedicated privacy, safety, and security professionals oversee cybersecurity risk management and mitigation, incident prevention, detection, and remediation. These teams comprise professionals with deep cybersecurity expertise across multiple industries and are led by our Vice President of Privacy, Safety, and Security, who has more than 20 years of experience, including roles in technology infrastructure for two other large public companies.
+Additionally, the Risk and Compliance Committee has oversight responsibility for risks and incidents relating to cybersecurity threats, and senior management regularly discusses cybersecurity risks and trends with this committee. Internal Audit also maintains a dedicated cybersecurity auditing team that independently tests our cybersecurity controls.
+[1], [2], [4], [5], and [6] all support this answer, highlighting the various teams and committees involved in overseeing cybersecurity at Alphabet.</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -695,7 +692,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>11.85</v>
+        <v>10.7</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -721,18 +718,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Alphabet faces several intellectual property risks, including:
-1. Inadequate protection of proprietary rights in certain countries where products and services are distributed or made available through the Internet.
-2. Risks associated with trade secrets, such as the confidentiality of sensitive information being compromised, which could result in losing competitive advantage (Source: [3] [4]).
-3. Uncertainty surrounding trademark protection, particularly if other courts outside of the US reach a different determination, potentially leading to loss of trademark protection for the "Google" brand.
-4. Increased risk of patent, copyright, trade secret, and trademark infringement lawsuits, which could result in awards of substantial monetary damages, costly royalty or licensing agreements, or orders preventing the company from offering certain features or products (Source: [5] [6]).
-5. Potential impact on business operations if injunctions are issued, leading to loss of revenues and adverse effects on the business.
-Overall, Alphabet faces a range of intellectual property risks that could have significant impacts on its business operations and financial results.
+          <t>Alphabet faces various intellectual property risks, including:
+1. Patent and trademark infringement lawsuits: Alphabet has had patent, copyright, trade secret, and trademark infringement lawsuits filed against them claiming that certain of their products, services, and technologies infringe others' intellectual property rights. [3]
+2. Loss of control over proprietary technology: Alphabet may lose control over its proprietary technology due to unauthorized use or disclosure, which could harm its business. [2]
+3. Infringement of trade secrets: The confidentiality of Alphabet's trade secrets and other sensitive information could be compromised, resulting in a loss of competitive advantage. [2]
+4. Risks associated with trademarks: Alphabet faces risks associated with its trademarks, such as the risk that the word "Google" becomes synonymous with the word "search." [2]
+5. Uncertainty around laws and regulations: The applicability and scope of laws and regulations relating to intellectual property, data protection, cybersecurity, and other areas are uncertain and could be interpreted in ways that harm Alphabet's business. [5]
+These risks could result in significant financial losses, reputational damage, or even loss of access to certain markets if Alphabet is unable to protect its intellectual property rights effectively.
 References:
-[3] Alphabet Inc. (GOOGL). Item 1A Risk Factors. Annual Report on Form 10-K.
-[4] Alphabet Inc. (GOOGL). Item 1A Risk Factors. Annual Report on Form 10-K.
-[5] Alphabet Inc. (GOOGL). Patent and Intellectual Property Claims. Quarterly Report on Form 10-Q.
-[6] Alphabet Inc. (GOOGL). Patent and Intellectual Property Claims. Quarterly Report on Form 10-Q.</t>
+[2] Alphabet Inc.'s 10-K filing with the SEC (2022)
+[3] Alphabet Inc.'s 10-K filing with the SEC (2022)
+[5] Alphabet Inc.'s 10-Q filing with the SEC (2022)</t>
         </is>
       </c>
       <c r="C8" t="n">
@@ -744,7 +740,7 @@
         </is>
       </c>
       <c r="E8" t="n">
-        <v>18.23</v>
+        <v>14.32</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -767,11 +763,20 @@
       <c r="B9" t="inlineStr">
         <is>
           <t>Alphabet faces various regulatory risks, including:
-1. Cybersecurity threats: The company has a dedicated cybersecurity auditing team that independently tests its cybersecurity controls, but it still faces the risk of material incidents and their impact on financial and other risks.
-2. Intellectual property claims: Alphabet is subject to patent, copyright, trade secret, and trademark infringement lawsuits, which could result in substantial monetary damages, costly royalty or licensing agreements, or orders preventing it from offering certain features or products (References [3] and [4]).
-3. Evolving laws and regulations: The company faces scrutiny from governments around the world with respect to its compliance with laws and regulations covering a wide variety of subjects, including AI, competition, consumer protection, content moderation, data privacy and security, intellectual property, news publications, and sustainability (References [5] and [6]).
-4. Increased enforcement actions and investigations: The company has seen an increase in new and evolving laws and regulations being proposed and implemented, as well as related enforcement actions and investigations, which could impact its business operations (Reference [5]).
-Overall, Alphabet's regulatory risks are diverse and complex, and the company must navigate a rapidly changing landscape of laws and regulations to minimize its exposure to potential risks.</t>
+1. Cybersecurity threats: Alphabet is subject to regulations related to cybersecurity, such as the General Data Protection Regulation (GDPR) in the EU and the California Consumer Privacy Act (CCPA) in the US [3].
+2. Intellectual property infringement: Alphabet may face lawsuits for patent, copyright, trade secret, and trademark infringement, which could result in costly royalty or licensing agreements, awards of substantial monetary damages, or orders preventing them from offering certain features or services [2].
+3. Competition and technology platforms' business practices: Alphabet is subject to laws and regulations related to competition and technology platforms' business practices, such as the Digital Markets Act in the EU and the Act on Promotion of Competition for Specified Smartphone Software in Japan [4].
+4. Data privacy and security: Alphabet's development, use, and commercialization of AI products and services may subject them to regulatory action and legal liability under laws such as data protection, cybersecurity, and intellectual property laws [6].
+5. Environmental sustainability and climate change: Alphabet is subject to evolving laws, regulations, policies, and international accords relating to environmental sustainability and climate change, which require significant investments in reporting frameworks and initiatives [6].
+6. Employment matters: Alphabet is also subject to regulations related to employment matters, such as labor laws and human capital management.
+7. Online content moderation: Alphabet may face regulatory risks related to online content moderation, including access restrictions for minors, consumer protection, and content moderation policies.
+These regulatory risks may result in substantial fines and penalties, injunctive relief, ongoing monitoring and auditing obligations, changes to their products and services, alterations to their business models and operations, including divestiture, and collateral-related civil litigation or other adverse consequences [5].
+References:
+[2] Alphabet. (Date). Patent and Intellectual Property Claims.
+[3] Alphabet. (Date). Digital Millennium Copyright Act and Section 230 of the Communications Decency Act in the US and the Digital Services Act in Europe.
+[4] Alphabet. (Date). Competition and technology platforms' business practices: Laws and regulations focused on large technology platforms, including the Digital Markets Act in the EU and the Act on Promotion of Competition for Specified Smartphone Software in Japan.
+[5] Alphabet. (Date). Various laws, regulations, investigations, enforcement lawsuits, and regulatory actions have involved in the past, and may in the future result in substantial fines and penalties, injunctive relief, ongoing monitoring and auditing obligations, changes to our products and services, alterations to our business models and operations, including divestiture, and collateral-related civil litigation or other adverse consequences.
+[6] Alphabet. (Date). Environmental sustainability and climate change: Legislation or court rulings affecting statutory safe harbors may harm us and may impose significant operational challenges.</t>
         </is>
       </c>
       <c r="C9" t="n">
@@ -783,7 +788,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>17.12</v>
+        <v>21.93</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -805,9 +810,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alphabet generates advertising revenue through performance and brand advertising. [1] Performance advertising revenues are recognized when a user engages with the advertisement, while brand advertising revenues are recognized when the ad is displayed or viewed. For ads placed on Google Network properties, Alphabet evaluates whether it is the principal (reporting revenues on a gross basis) or agent (reporting revenues on a net basis). [1] Where Alphabet is the principal, it controls the advertising inventory before transferring it to customers and recognizes revenues from amounts billed to customers as revenue. [1]
-Additionally, Alphabet's Google Subscriptions, Platforms, and Devices segment generates revenue from consumer subscriptions and platforms. Consumer subscriptions primarily include revenues from YouTube services such as YouTube TV, YouTube Music, and Premium, as well as Google One, which offers access to its most capable Gemini models. [4] The platforms segment includes other platforms that generate advertising revenues for Alphabet.
-It's worth noting that the exact breakdown of revenue streams is not specified in the provided context, but it gives an idea of how Alphabet generates advertising revenue through performance and brand advertising on Google Network properties, as well as through consumer subscriptions and platforms.</t>
+          <t>Alphabet generates advertising revenue through delivering both performance and brand advertising. Specifically, for ads placed on Google Network properties, they evaluate whether they are the principal or agent, generally reporting revenues on a gross basis. This means that when amounts billed to customers are recorded as revenues, and amounts paid to Google Network partners are recorded as cost of revenues.
+Alphabet's advertising revenue consists of:
+1. Revenues from YouTube services, such as YouTube TV, YouTube Music and Premium, and NFL Sunday Ticket, as well as Google One.
+2. Revenues from platforms, which primarily include advertising on Google-owned properties like Gmail, Google Maps, and Google Play.
+3. Sales of other products and services, including subscription-based products, apps and in-app purchases, and devices.
+(References: [1], [2], [5])</t>
         </is>
       </c>
       <c r="C10" t="n">
@@ -819,7 +827,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>17.32</v>
+        <v>11.73</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -841,12 +849,13 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Alphabet's cloud business is referred to as Google Cloud. According to sources [2] and [5], Alphabet reports its cloud-based solutions that provide enterprise customers with infrastructure, platform services, and applications under the segment "Google Cloud".
-Source: [2]
-a collection of businesses — the largest of which is Google. We report Google in two segments, Google Services and Google Cloud, and all non-Google businesses collectively as Other Bets.
-And also, according to source [5]:
-We generate revenues by delivering relevant, cost-effective online advertising; cloud-based solutions that provide enterprise customers of all sizes with infrastructure, platform services, and applications; and sales of other products and services, such as fees received for subscription-based products, apps and in-app purchases, and devices.
-Note: Alphabet's cloud business is also mentioned in source [6], which appears to be a duplicate of sources [2] and [5].</t>
+          <t>Alphabet's cloud business, also known as Google Cloud, generates revenues primarily from consumption-based fees and subscriptions received for infrastructure and platform services, applications, and other services for enterprise customers. [6] According to Google, "Google Cloud Platform primarily generates consumption-based fees and subscriptions for infrastructure, platform, and other services." [4]
+Google Cloud includes various services such as:
+* Infrastructure and platform services
+* Applications
+* Other enterprise services
+These services provide access to solutions such as AI offerings, cybersecurity offerings, and data and analytics solutions. [4] Google Cloud also offers communication and collaboration tools for enterprises, including Gmail, Docs, Calendar, Drive, and Meet, with integrated features like Gemini for Google Workspace. [4]
+Revenues from Google Cloud are generated primarily from consumption-based fees and subscriptions received for Google Cloud Platform services, Google Workspace communication and collaboration tools, and other enterprise services.</t>
         </is>
       </c>
       <c r="C11" t="n">
@@ -858,7 +867,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>16.25</v>
+        <v>11.92</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -880,19 +889,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Based on the provided context, Alphabet Inc.'s (formerly Google) main products and services include:
-1. Online advertising
-2. Cloud-based solutions for enterprise customers, including infrastructure, platform services, and applications
-3. Sales of other products and services, such as:
-	* Subscription-based products, apps, and in-app purchases
-	* Devices
-These are mentioned in [5] (GOOGL), which provides an overview of Alphabet's revenue streams.
-Additionally, Alphabet has a range of other businesses, including:
-1. Google Services and Google Cloud segments
-2. Other Bets, which includes non-Google businesses
-3. AI-related research and development, reported in Alphabet-level activities
-These are mentioned in [3] (GOOGL), which provides an overview of Alphabet's structure and businesses.
-Please note that the context provided does not provide a comprehensive list of Alphabet's main products and services, but rather highlights some of the key revenue streams and business areas.</t>
+          <t>Alphabet's main products and services include:
+1. Online advertising: Alphabet generates revenues by delivering relevant, cost-effective online advertising (Source: [3])
+2. Cloud-based solutions: The company provides enterprise customers with infrastructure, platform services, and applications (Source: [3])
+3. Sales of other products and services: Alphabet also sells other products and services, such as fees received for subscription-based products, apps, and in-app purchases, and devices (Source: [3])
+In addition to these main products and services, Alphabet has various other businesses, including Google Services, Google Cloud, and Other Bets (Source: [2]).</t>
         </is>
       </c>
       <c r="C12" t="n">
@@ -904,7 +905,7 @@
         </is>
       </c>
       <c r="E12" t="n">
-        <v>16.47</v>
+        <v>10.67</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -926,13 +927,9 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided context does not explicitly mention Alphabet's geographic regions of operation. However, based on general knowledge and available information, I can provide some insights.
-Alphabet Inc., the parent company of Google, operates globally with a presence in various countries around the world. According to Alphabet's annual reports and public statements, they have a significant presence in:
-1. North America: The United States and Canada.
-2. Europe: The UK, Germany, France, and other European countries.
-3. Asia-Pacific: Japan, Australia, China (through its subsidiaries), and other Asian countries.
-It is worth noting that Alphabet's operations are not limited to these regions, as they have a global presence through their various businesses, including Google Cloud, YouTube, and Android.
-If you need more specific information on Alphabet's geographic regions of operation, I suggest checking their official website or annual reports for more detailed information.</t>
+          <t>Unfortunately, the provided context does not explicitly state which geographic regions Alphabet operates in. However, based on [1] (GOOGL), we can infer that Google, a subsidiary of Alphabet, generates revenues by delivering online advertising, cloud-based solutions, and other products and services globally.
+While the exact geographic regions are not specified in the context provided, it is known that Alphabet Inc., formerly known as Google, operates in many countries around the world. 
+However, without more explicit information from Alphabet itself or another reliable source, it's difficult to pinpoint the specific geographic regions where Alphabet operates.</t>
         </is>
       </c>
       <c r="C13" t="n">
@@ -944,21 +941,17 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>16.47</v>
+        <v>10.74</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>geographic, region</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>revenue</t>
-        </is>
-      </c>
+          <t>geographic, revenue, region</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -970,13 +963,16 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Based on the provided context, Alphabet faces various antitrust or competition risks, including:
-1. Risk of losing intellectual property rights: The company acknowledges that effective intellectual property protection may not be available in every country where its products and services are distributed or made available through the Internet. Additionally, there is a risk that an issued patent may be deemed invalid or unenforceable.
-2. Potential trademark dilution: Alphabet notes that the word "Google" could become synonymous with the word "search," which could lead to a loss of protection for its trademark if other courts reach a different determination than US courts.
-3. Risk of patent infringement lawsuits: The company faces lawsuits claiming that certain of its products, services, and technologies infringe others' intellectual property rights. Adverse results in these lawsuits may include awards of substantial monetary damages or orders preventing the company from offering certain features or products.
-4. Potential prohibition on importing infringing products: A loss in an International Trade Commission (ITC) action can result in a prohibition on importing infringing products into the US, which could have an adverse effect on Alphabet's business.
-5. Risk of losing customers and partners due to injunctions: Injunctive orders against Alphabet's products or services may cause its customers and partners to discontinue use, leading to loss of revenues and harm to the company's business.
-These risks highlight the importance of protecting intellectual property rights, managing trademark portfolios, and navigating complex competition laws to avoid antitrust issues.</t>
+          <t>Alphabet faces several antitrust and competition risks, including:
+1. Antitrust lawsuits about aspects of its business, including its advertising technologies and practices, the operation and distribution of Google Search, and the operation and distribution of Android operating system and Play Store.
+[2], [4]
+2. Private individual and collective actions that overlap with claims pursued by regulatory authorities are pending in the US and in several other jurisdictions, including across Europe.
+[2], [5]
+3. Investigations and litigation related to its collection and use of location information, the choices it offers users, and advertising practices, which could result in significant fines, judgments, and product changes.
+[4]
+4. Preliminary findings of non-compliance by the European Commission (EC) regarding Google's compliance with certain provisions of the EU's Digital Markets Act relating to Google Play and Search.
+[6]
+These risks may require Alphabet to implement remedies, alter its business practices, and incur significant costs, which could harm its business, reputation, financial condition, and operating results.</t>
         </is>
       </c>
       <c r="C14" t="n">
@@ -988,7 +984,7 @@
         </is>
       </c>
       <c r="E14" t="n">
-        <v>20.27</v>
+        <v>13.81</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1010,12 +1006,22 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Based on the provided context, Alphabet faces several privacy risks, including:
-1. Data privacy and security concerns relating to their technology and practices, which could harm their reputation, cause significant liability, and deter users or customers from using their products and services.
-2. Concerns about the adequacy of their practices with regard to the collection, use, governance, disclosure, or security of personal data or other data-privacy-related matters, even if unfounded, which could harm their business, reputation, financial condition, and operating results.
-3. Malicious software such as viruses, software bugs, theft, misuse, defects, vulnerabilities in their products and services, as well as cyber attacks, phishing schemes, and other types of security attacks, which increasingly use AI, expose them to a risk of loss or improper use and disclosure of sensitive information.
-These risks are mentioned in [5] (GOOGL) and [6] (GOOGL), which highlight the potential consequences of data privacy and security breaches on Alphabet's business and reputation.
-Additionally, the context mentions that concerns about privacy practices could be unfounded but still have a negative impact on their business and operating results.</t>
+          <t>Alphabet faces various privacy risks, including:
+1. Risks related to the collection, use, governance, disclosure, or security of personal data, which could harm their business, reputation, financial condition, and operating results. [3]
+2. Concerns about the adequacy of their practices with regard to the collection, use, governance, disclosure, or security of personal data, even if unfounded, which could also harm their business, reputation, financial condition, and operating results. [3]
+3. Various US federal, US state, and foreign privacy laws related to the processing and security of personal data, including comprehensive privacy laws that provide data privacy rights and impose significant obligations on controllers and processors of consumer data. [4]
+4. The EU's Digital Markets Act, which requires companies to comply with privacy and data protection regulations. [5]
+5. The risk of unauthorized access to user data by third parties, including investigation and review of platform applications that could access the information of users of their services. [6]
+These risks include:
+* Cyber attacks, phishing schemes, and other types of security attacks, which increasingly use AI.
+* Malicious software such as viruses, software bugs, theft, misuse, defects, vulnerabilities in their products and services, as well as cyber attacks, which expose them to a risk of loss or improper use and disclosure of user data. [3]
+* False or undesirable user accounts, election interference, improper ad purchases, activities that threaten people's safety on- or off-line, or instances of spamming, scraping, or spreading disinformation. [6]
+Overall, Alphabet faces significant privacy risks that could harm their business, reputation, financial condition, and operating results if not addressed effectively.
+References:
+[3] (GOOGL)
+[4] (GOOGL)
+[5] (GOOGL)
+[6] (GOOGL)</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1027,7 +1033,7 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>16.83</v>
+        <v>19.44</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1049,18 +1055,20 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Alphabet, the parent company of Google, faces various litigation risks, including:
-1. **Cybersecurity threats**: The company may be subject to fines and penalties for unauthorized access to user data, failure to protect against cyber attacks, or other cybersecurity breaches [3].
-2. **Intellectual property infringement**: Alphabet has faced patent, copyright, trade secret, and trademark infringement lawsuits claiming that its products, services, and technologies infringe on others' intellectual property rights [5].
-3. **Regulatory actions**: The company may face regulatory actions, investigations, enforcement lawsuits, and sanctions for various legal theories, including unlawful activity, torts, privacy rights violations, fraud, or other legal theories based on the nature and content of information available on or via its services [1].
-4. **Data protection and privacy**: Alphabet may be subject to fines and penalties for non-compliance with data protection regulations, such as GDPR or CCPA.
-These litigation risks can have a significant impact on Alphabet's business, reputation, financial condition, and operating results.
+          <t>Alphabet faces a variety of litigation risks, including:
+1. Cybersecurity threats and related legal proceedings [2]
+2. Patent and intellectual property infringement lawsuits [3]
+3. Regulatory agency challenges to business practices and compliance with laws and regulations [4]
+4. Product warranty, product liability, and consumer protection claims related to product defects [4]
+5. Health and safety, hazardous materials usage, and environmental effects claims [6]
+6. Antitrust lawsuits regarding advertising technologies and practices, Google Search, Android operating system, and Play Store [6]
+These litigation risks may result in substantial fines, penalties, injunctive relief, ongoing monitoring and auditing obligations, changes to business models and operations, including divestiture, and collateral related civil litigation or other adverse consequences.
 References:
-[1] Alphabet Inc. (2022). 2022 Annual Report (Form 10-K). Retrieved from &lt;https://www.google.com/corporate/financials&gt;
-[2] Alphabet Inc. (2022). 2022 Annual Report (Form 10-K). Retrieved from &lt;https://www.google.com/corporate/financials&gt;
-[3] Alphabet Inc. (2022). Cybersecurity Disclosure Statement. Retrieved from &lt;https://www.google.com/corporate/cybersecurity-disclosure-statement/&gt;
-[4] Alphabet Inc. (2022). Risk and Compliance Committee Charter. Retrieved from &lt;https://www.google.com/corporate/risk-and-compliance-committee-charter/&gt;
-[5] Alphabet Inc. (2022). Patent and Intellectual Property Claims. Retrieved from &lt;https://www.google.com/corporate/patent-and-intellectual-property-claims/&gt;</t>
+[2] Alphabet Inc. Form 10-K for the year ended December 31, 2022, Item 3. Legal Proceedings.
+[3] Alphabet Inc. Form 10-K for the year ended December 31, 2022, Item 8. Financial Information and Reporting of Non-GAAP Measures.
+[4] Alphabet Inc. Form 10-K for the year ended December 31, 2022, Item 1. Business.
+[5] Alphabet Inc. Form 10-K for the year ended December 31, 2022, Item 3. Legal Proceedings.
+[6] Alphabet Inc. Form 10-K for the year ended December 31, 2022, Item 8. Financial Information and Reporting of Non-GAAP Measures.</t>
         </is>
       </c>
       <c r="C16" t="n">
@@ -1072,7 +1080,7 @@
         </is>
       </c>
       <c r="E16" t="n">
-        <v>22.91</v>
+        <v>17.85</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1094,9 +1102,10 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided text does not explicitly mention Alphabet's capital commitments.
-However, based on the context, it appears that Alphabet regularly evaluates its cash and capital structure, including the size, pace, and form of capital return to stockholders. This suggests that Alphabet has made certain financial commitments or investments, but this information is not explicitly stated in the provided text.
-To answer your question more accurately, I would need access to additional sources or context that specifically mention Alphabet's capital commitments. If you could provide more information or clarify what you are looking for, I'll do my best to assist you.</t>
+          <t>Unfortunately, the provided context does not mention Alphabet's capital commitments. The text appears to be a snippet from Alphabet Inc.'s annual report or financial statements, but it does not provide information on the company's capital commitments.
+However, based on Alphabet's stock purchases and investments in various entities, it is possible to make an educated guess about their capital commitments. According to Alphabet's annual reports and financial statements, the company has made significant investments in various projects, such as self-driving cars, artificial intelligence, and renewable energy (e.g., [1]).
+Additionally, Alphabet has also committed to certain milestones and targets for its various businesses, such as Google Cloud and YouTube Premium (e.g., [2]). However, without more specific information, it is difficult to determine the exact amount of Alphabet's capital commitments.
+If you have any further context or clarify what you mean by "capital commitments," I may be able to provide a more specific answer.</t>
         </is>
       </c>
       <c r="C17" t="n">
@@ -1108,7 +1117,7 @@
         </is>
       </c>
       <c r="E17" t="n">
-        <v>13.05</v>
+        <v>14.17</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1130,20 +1139,18 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Alphabet has a multi-layered approach to managing data security, which includes:
-1. Remediation and resolution of incidents: Alphabet has a cross-functional working group that reviews significant incidents regularly to determine whether further escalation is appropriate. Any incident assessed as potentially being or potentially becoming material is promptly escalated for further assessment, and then reported to designated members of senior management [2].
-2. Cybersecurity audits: Internal Audit maintains a dedicated cybersecurity auditing team that independently tests Alphabet's cybersecurity controls [2].
-3. Risk and Compliance Committee oversight: The Risk and Compliance Committee has oversight responsibility for risks and incidents relating to cybersecurity threats, including compliance with disclosure requirements, cooperation with law enforcement, and related effects on financial and other risks [2].
-4. Use of outside counsel: Alphabet consults with outside counsel as appropriate, including on materiality analysis and disclosure matters [2].
-5. Maintenance of security protections: Alphabet expects to continue expending significant resources to maintain security protections that limit the effect of bugs, theft, misuse, and security vulnerabilities or breaches [3].
-Alphabet also acknowledges the risks associated with its business, including:
-1. Malicious software and cyber attacks: Alphabet's products and services involve the storage, handling, and transmission of proprietary and other sensitive information, which exposes it to a risk of loss or improper use and disclosure of such information [3].
-2. AI-centric security risks: Alphabet's products incorporate highly technical and complex technologies, and thus its technologies and software have contained, and are likely in the future to contain, undetected errors, bugs, or vulnerabilities [3].
-3. Regulatory and legal exposure: Systems and control failures, security breaches, failure to comply with privacy policies, and inadvertent disclosure of user data could result in regulatory and legal exposure [3].
-Overall, Alphabet has a robust approach to managing data security, but acknowledges that there are risks associated with its business and is committed to continuing to expend significant resources to maintain security protections.
+          <t>Alphabet has a comprehensive process for identifying, assessing, and managing material risks from cybersecurity threats as part of its broader risk management system and processes. [4] The company maintains a dedicated cybersecurity auditing team that independently tests its cybersecurity controls. [2]
+The Risk and Compliance Committee oversees risks and incidents relating to cybersecurity threats, including compliance with disclosure requirements, cooperation with law enforcement, and related effects on financial and other risks. [1] Senior management regularly discusses cybersecurity risks and trends with the Risk and Compliance Committee, and the executive leadership team is responsible for the overall enterprise risk management system and processes.
+Alphabet also consults with outside counsel as appropriate, including on materiality analysis and disclosure matters, and its senior management makes the final materiality determinations and disclosure decisions. [1]
+In addition, Alphabet has invested significant resources in safety, security, and review efforts to combat misuse of its services and unauthorized access to user data by third parties. [5] The company has also made investments in AI technologies that rely on the collection of large amounts of data, and it is aware of the need for evolving interpretations of data protection regulations. [6]
+Overall, Alphabet's approach to managing data security appears to involve a combination of proactive measures, such as investing in cybersecurity controls and review efforts, as well as reactive measures, such as responding quickly to incidents and cooperating with law enforcement. However, it is worth noting that no company can guarantee that it will not experience significant damage from cyber attacks or other cybersecurity threats.
 References:
-[2] Alphabet Inc. (2022). 2022 Form 10-K for the Year Ended December 31, 2021.
-[3] Alphabet Inc. (2022). Alphabet Inc. Restated Consolidated Financial Statements (Form 10-K)</t>
+[1] Alphabet Inc.'s 2022 Form 10-K
+[2] Alphabet Inc.'s 2022 Annual Report on Form 10-K
+[3] Alphabet Inc.'s Basis of Consolidation
+[4] Alphabet Inc.'s Use of Estimates and Management's Discussion and Analysis
+[5] Alphabet Inc.'s Safety, Security, and Content Review Efforts
+[6] Alphabet Inc.'s Risks Related to Laws, Regulations, and Policies</t>
         </is>
       </c>
       <c r="C18" t="n">
@@ -1155,7 +1162,7 @@
         </is>
       </c>
       <c r="E18" t="n">
-        <v>22.99</v>
+        <v>26.39</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1177,9 +1184,18 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Alphabet faces third-party risks including cybersecurity threats, nation-states and state-sponsored actors, employee or insider error or malfeasance, system errors, vulnerabilities in its or other parties' systems, various laws and regulations, investigations, enforcement lawsuits, and regulatory actions. [3], [4], [5]
-These risks may result in significant legal, financial, and reputational harm, including government inquiries, enforcement actions, litigation, negative publicity, substantial fines and penalties, injunctive relief, ongoing monitoring and auditing obligations, changes to its products and services, alterations to its business models and operations, divestiture, civil litigation or other adverse consequences. [5], [6]
-Alphabet also expects to continue to experience incidents or vulnerabilities in the future due to the nature of its business, which involves hosting, transmitting, marketing, branding, and providing access to content created by third parties.</t>
+          <t>Alphabet faces various third-party risks, including:
+1. Nation-state and state-sponsored actors' cyber attacks and data exfiltration or compromise ([2])
+2. Cybersecurity threats from employees or insider error or malfeasance, system errors, or vulnerabilities in our or other parties' systems ([3])
+3. Unauthorized use of intellectual property rights by third parties ([5])
+4. Malicious software such as viruses, software bugs, theft, misuse, defects, vulnerabilities in our products and services, as well as cyber attacks, phishing schemes, and other types of security attacks ([6])
+These risks can harm Alphabet's business, reputation, financial condition, and operating results, and may result in significant legal, financial, and reputational harm.
+References:
+[2] (GOOGL)
+[3] (GOOGL)
+[4] (GOOGL)
+[5] (GOOGL)
+[6] (GOOGL)</t>
         </is>
       </c>
       <c r="C19" t="n">
@@ -1191,7 +1207,7 @@
         </is>
       </c>
       <c r="E19" t="n">
-        <v>8.82</v>
+        <v>13.92</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1213,9 +1229,9 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>The Risk and Compliance Committee has oversight responsibility for risks and incidents relating to cybersecurity threats, including compliance with disclosure requirements, cooperation with law enforcement, and related effects on financial and other risks. They report any findings and recommendations as appropriate to the full Board for consideration.
-[1], [3], [4], and [6] (GOOGL) all cite this information.
-Additionally, it is mentioned that the Risk and Compliance Committee has oversight responsibility for cybersecurity threats, but no specific information is provided about their role in managing or mitigating these risks.</t>
+          <t>The Risk and Compliance Committee has oversight responsibility for risks and incidents relating to cybersecurity threats, including compliance with disclosure requirements, cooperation with law enforcement, and related effects on financial and other risks. It reports any findings and recommendations, as appropriate, to the full Board for consideration.
+Additionally, senior management regularly discusses cybersecurity risks and trends and, should they arise, any material incidents with the Risk and Compliance Committee. Internal Audit maintains a dedicated cybersecurity auditing team that independently tests our cybersecurity controls (References [2] and [4]).
+The Risk and Compliance Committee also has responsibility for reporting to the full Board of Directors on cybersecurity matters (Reference [6]).</t>
         </is>
       </c>
       <c r="C20" t="n">
@@ -1227,7 +1243,7 @@
         </is>
       </c>
       <c r="E20" t="n">
-        <v>7.45</v>
+        <v>10.87</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1249,13 +1265,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Alphabet faces scrutiny from both US and foreign governments with respect to its compliance with laws and regulations, particularly in areas such as AI, competition, consumer protection, content moderation, data privacy and security, intellectual property, news publications, and sustainability and other social matters.
-Specifically, Alphabet has faced:
-* Increasingly heightened scrutiny from the US government regarding its compliance with federal, state, and local laws and regulations [3]
-* Foreign governments' scrutiny of the company's compliance with international laws and regulations [3]
-* Investigations and enforcement actions by legislative and regulatory bodies around the world [3]
-These inquiries and regulatory developments may impact Alphabet's business strategy, results of operations, and financial condition.
-Note: The question is not specific about a particular government or regulatory inquiry, but rather implies that Alphabet faces scrutiny from multiple governments and regulatory bodies.</t>
+          <t>Alphabet faces numerous government and regulatory inquiries, including:
+* Scrutiny from both US and foreign governments regarding compliance with laws and regulations [2]
+* Increased enforcement actions and investigations by legislative and regulatory bodies around the world, particularly in areas such as AI, competition, consumer protection, content moderation, data privacy and security, intellectual property, news publications, and sustainability [2]
+* Registration statements (Form S-3, S-8, etc.) related to various stock plans, indicating that Alphabet is subject to ongoing regulatory scrutiny with regards to its equity compensation practices [6]
+Note: The information provided in this answer is based on the context of Alphabet's risk management and compliance processes, as well as its regulatory filings.</t>
         </is>
       </c>
       <c r="C21" t="n">
@@ -1267,17 +1281,21 @@
         </is>
       </c>
       <c r="E21" t="n">
-        <v>8.9</v>
+        <v>11.61</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>government, regulatory, inquiry</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr"/>
+          <t>government, regulatory</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>inquiry</t>
+        </is>
+      </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
     </row>
@@ -1289,13 +1307,9 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Based on the provided context, it appears that Alphabet's management has access to multiple sources of expertise in cybersecurity. While no specific examples are mentioned, it is stated that:
-* Teams of dedicated privacy, safety, and security professionals oversee cybersecurity risk management and mitigation, incident prevention, detection, and remediation.
-* These teams comprise professionals with deep cybersecurity expertise across multiple industries.
-* The Vice President of Privacy, Safety, and Security has more than 20 years of experience in technology infrastructure for two other large public companies.
-Therefore, it can be inferred that Alphabet's management has access to a diverse range of cybersecurity expertise through its internal teams and external experts. However, no specific details are provided about the individual skills or qualifications of the senior management team members.
-References:
-[1], [2], [3], [4], [5]</t>
+          <t>Alphabet's management has deep cybersecurity expertise across multiple industries, led by their Vice President of Privacy, Safety, and Security, who has more than 20 years of experience, including roles in technology infrastructure for two other large public companies [2], [3], [5].
+In particular, the teams that oversee cybersecurity risk management and mitigation, incident prevention, detection, and remediation comprise professionals with deep cybersecurity expertise across multiple industries. These teams are led by the Vice President of Privacy, Safety, and Security, who has extensive experience in technology infrastructure for two other large public companies [2], [3], [5].
+Additionally, Alphabet's executive leadership team regularly considers cybersecurity risks in the context of other material risks to the company, and senior management discusses cybersecurity risks and trends with the Risk and Compliance Committee [4].</t>
         </is>
       </c>
       <c r="C22" t="n">
@@ -1307,7 +1321,7 @@
         </is>
       </c>
       <c r="E22" t="n">
-        <v>11.42</v>
+        <v>13.6</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -1330,13 +1344,12 @@
       <c r="B23" t="inlineStr">
         <is>
           <t>Alphabet's revenue streams include:
-1. Online advertising
-2. Cloud-based solutions
-3. Subscription-based products, apps, and in-app purchases
-4. Devices
-These revenue streams come from various segments of the company, including Google and Other Bets. The specific revenue streams for each segment are not separately disclosed in the provided context.
-According to Alphabet's annual report, they generate revenues through delivering relevant, cost-effective online advertising; cloud-based solutions that provide enterprise customers with infrastructure, platform services, and applications; and sales of other products and services, such as fees received for subscription-based products, apps, and devices. [5]
-Additionally, Alphabet's Other Bets segment generates revenue primarily from the sale of autonomous transportation services and internet services. [1]</t>
+1. Advertising revenues from Google Search and other properties, including traffic generated by search distribution partners [5].
+2. Revenues from YouTube services, such as YouTube TV, YouTube Music and Premium, and NFL Sunday Ticket, as well as Google One, which offers access to Alphabet's most capable Gemini models (consumer subscriptions) [4].
+3. Revenues from cloud-based solutions that provide enterprise customers with infrastructure, platform services, and applications [3].
+4. Sales of other products and services, such as fees received for subscription-based products, apps and in-app purchases, and devices [3].
+5. Revenues from autonomous transportation services and internet services, primarily generated by Alphabet's investment in the portfolio of Other Bets [6].
+Note: Other Bets include businesses that are at various stages of development, ranging from research and development phase to commercialization, such as Waymo, X, and others [6].</t>
         </is>
       </c>
       <c r="C23" t="n">
@@ -1348,7 +1361,7 @@
         </is>
       </c>
       <c r="E23" t="n">
-        <v>12.15</v>
+        <v>13.88</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -1370,8 +1383,14 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>According to sources [2] and [4], YouTube provides people with entertainment, information, and opportunities to learn something new, and helps support the creator economy through the YouTube Partner Program. Additionally, according to source [5], YouTube is a part of Alphabet's revenue generation stream, alongside other products and services such as online advertising, cloud-based solutions, subscription-based products, apps, in-app purchases, and devices.
-In particular, source [2] states that "YouTube provides people with entertainment, information, and opportunities to learn something new and helps support the creator economy through the YouTube Partner Program."</t>
+          <t>According to Alphabet's annual report, YouTube is one of the businesses that make up Alphabet Inc., along with Google. [2] YouTube provides people with entertainment, information, and opportunities to learn something new.
+Additionally, YouTube is part of Alphabet's "Access and Technology for Everyone" mission, which aims to make technology accessible and useful to everyone. [2]
+YouTube also generates revenue through advertising, similar to other parts of Alphabet's business, such as Google. [5] The report states that YouTube properties, including revenues from AdMob, AdSense, and Google Ad Manager, are included in Alphabet's revenue. [4]
+Therefore, YouTube plays a significant role in Alphabet's business, providing entertainment, information, and advertising revenue.
+References:
+[2] (GOOGL)
+[4] (GOOGL)
+[5] (GOOGL)</t>
         </is>
       </c>
       <c r="C24" t="n">
@@ -1383,7 +1402,7 @@
         </is>
       </c>
       <c r="E24" t="n">
-        <v>12.53</v>
+        <v>13.55</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -1405,19 +1424,16 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Alphabet Inc.'s main risk factors include:
-1. Cybersecurity threats and vulnerabilities, including the potential for cyber attacks and data exfiltration or compromise by nation-states and state-sponsored actors.
-2. Geopolitical tensions or armed conflicts, which may increase the risks of cyber attacks.
-3. Security and privacy issues due to employee or insider error or malfeasance, system errors, or vulnerabilities in their systems.
-These risk factors are mentioned in Alphabet's annual reports and SEC filings, including their Form 10-K for the year ended December 31, 2022 [1], [2], [4], [5].
-Specifically, Alphabet notes that they expect to continue to experience cybersecurity incidents or vulnerabilities in the future, which could require additional resources to prepare and defend against such threats [1]. They also acknowledge the risk of cyber attacks and data exfiltration or compromise by nation-states and state-sponsored actors, particularly targeting their public sector customers [2].
-Additionally, Alphabet notes that security and privacy issues can arise due to various factors, including employee or insider error or malfeasance, system errors, or vulnerabilities in their systems [4]. These issues may result in significant legal, financial, and reputational harm, including government inquiries, enforcement actions, litigation, and negative publicity.
-References:
-[1] Alphabet Inc. (2022). Form 10-K for the year ended December 31, 2022. Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1302235/000110465920222154/abcde1234.pdf&gt;
-[2] Alphabet Inc. (2022). Alphabet's Risk Management Framework. Retrieved from &lt;https://about.alphabet.com/risk-management/&gt;
-[3] Alphabet Inc. (n.d.). Cybersecurity. Retrieved from &lt;https://www.alphabeat.com/cybersecurity/&gt;
-[4] Alphabet Inc. (2022). Form 10-K for the year ended December 31, 2022. Retrieved from &lt;https://www.sec.gov/Archives/edgar/data/1302235/000110465920222155/abcde1234.pdf&gt;
-[5] Alphabet Inc. (n.d.). National Cybersecurity. Retrieved from &lt;https://about.alphabet.com/cybersecurity/national-cybersecurity/&gt;</t>
+          <t>Alphabet's main risk factors include:
+1. Cybersecurity threats, such as data breaches and intellectual property theft, which could lead to significant legal, financial, and reputational harm. [2]
+2. Foreign exchange risk related to the remeasurement of monetary assets or liabilities denominated in currencies other than the functional currency of a subsidiary. [5]
+3. Other risks, including the impact of geopolitical tensions or armed conflicts on cybersecurity threats and data exfiltration or compromise by nation-states and state-sponsored actors. [2]
+4. Material incidents, such as significant breaches or vulnerabilities, which could affect Alphabet's systems and potentially materialize into significant financial or reputational harm. [1]
+These risks are managed through various means, including:
+* A comprehensive cybersecurity risk management process that includes incident response, threat intelligence, and regular reviews of risks and incidents. [2]
+* Derivatives to manage foreign exchange risk and other risks, such as data center leases. [5]
+* Regular discussions between senior management and the Risk and Compliance Committee on cybersecurity risks and trends. [1]
+Overall, Alphabet's main risk factors are cybersecurity threats, including material incidents, foreign exchange risk, and other risks related to geopolitics and nation-state attacks.</t>
         </is>
       </c>
       <c r="C25" t="n">
@@ -1429,7 +1445,7 @@
         </is>
       </c>
       <c r="E25" t="n">
-        <v>27.47</v>
+        <v>16.22</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -1451,9 +1467,10 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Alphabet mentions the risk of cyber attacks and data exfiltration or compromise by nation-states and state-sponsored actors, particularly in relation to its public sector customers (including federal, state, and local governments) [2]. It also notes that geopolitical tensions or armed conflicts, such as the ongoing conflict in the Middle East and Ukraine, may increase these risks [2].
-Additionally, Alphabet mentions that cyber attacks by nation-states can target their employees or impersonate members of senior management to gain unauthorized access to their systems [3]. 
-There is no specific mention of which nation-state, but it does discuss general nation-state threats as a whole.</t>
+          <t>Alphabet mentions the risk of cyber attacks and data exfiltration or compromise by nation-states and state-sponsored actors, particularly in their public sector customers (including federal, state, and local governments) [1]. They also mention that geopolitical tensions or armed conflicts, such as the ongoing conflict in the Middle East and Ukraine, may increase these risks [1].
+There is no specific nation-state mentioned in the text, but it can be inferred that Alphabet is concerned about the risk of cyber attacks from various nation-states and state-sponsored actors.
+References:
+[1] (GOOGL)</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1465,7 +1482,7 @@
         </is>
       </c>
       <c r="E26" t="n">
-        <v>15.19</v>
+        <v>11.72</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -1487,13 +1504,19 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Unfortunately, there isn't enough text provided in your question to give me a clear answer about what you're looking for. Based on the context of your question I can only try and make an educated guess.
-If we look at what is being discussed in [3], [4], [5] and [6], it appears that these are all describing how Apple recognizes revenue, which could be a risk factor.
-These factors include:
-* Regulatory requirements: This is mentioned in [3].
-* Compliance with competition-related laws and regulations: This is mentioned in [3] and [4].
-* Uncertainty over pricing for similar offerings, product-specific business objectives, and the estimated cost to provide performance obligations: These are all discussed in [5] and [6].
-Please let me know if any of these seem relevant to your question.</t>
+          <t>Based on the provided context, Apple's main risk factors include:
+1. Compliance with regulatory requirements, including competition-related laws and regulations in various jurisdictions. This includes the Digital Markets Act (DMA) in the EU, which imposes wide-ranging obligations on technology companies, including significant limitations on businesses like Apple.
+2. Investigations and litigation related to antitrust laws, such as U.S. antitrust lawsuits alleging monopolization or attempted monopolization in the markets for "performance smartphones" and "smartphones," and investigations in Europe and other jurisdictions relating to App Store terms and conditions.
+3. Commercial relationships with other companies that are or may become subject to investigations and litigation, which could materially adversely affect Apple's commercial relationships and business results.
+4. Government investigations and legal proceedings related to licensing arrangements with Google LLC, such as the recent finding of U.S. antitrust law violations by Google and the subsequent court order requiring certain remedies.
+These risk factors are mentioned in the context of Apple's Annual Report (Form 10-K) for the year ended September 27, 2025, which includes the opinion of Ernst &amp; Young LLP on internal control over financial reporting.
+References:
+[1] AAPL. (2025). Compensation Plan.
+[2] AAPL. (2025). Regulatory requirements.
+[3] AAPL. (2025). Performance obligations.
+[4] AAPL. (2025). Company background and risks.
+[5] AAPL. (2025). Trust lawsuit risks.
+[6] AAPL. (2025). Opinion on internal control over financial reporting.</t>
         </is>
       </c>
       <c r="C27" t="n">
@@ -1505,7 +1528,7 @@
         </is>
       </c>
       <c r="E27" t="n">
-        <v>16.72</v>
+        <v>18.43</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -1527,14 +1550,16 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>The question does not provide enough context to determine which specific reportable segments Apple has. However, based on the provided XML data, I can identify some of the reportable segments and their associated roles.
-From the XML data, we can see that there are at least two reportable segments:
-1. "Segment Information and Geographic Data" (http://www.apple.com/role/SegmentInformationandGeographicData)
-2. "Revenue - Disaggregated Net Sales and Portion of Net Sales That Was Previously Deferred" (http://www.apple.com/role/RevenueDisaggregatedNetSalesandPortionofNetSalesThatWasPreviouslyDeferredDetails)
-These segments are associated with specific reports, such as:
-* "Segment Information and Geographic Data (Tables)" (http://www.apple.com/role/SegmentInformationandGeographicDataTables)
-* "Revenue - Disaggregated Net Sales and Portion of Net Sales That Was Previously Deferred (Details)" (http://www.apple.com/role/RevenueDisaggregatedNetSalesandPortionofNetSalesThatWasPreviouslyDeferredDetails)
-Please note that this is not an exhaustive list, and there may be other reportable segments not included in the provided XML data.</t>
+          <t>Unfortunately, the provided context does not explicitly state what Apple's reportable segments are. However, based on the information available in the context, we can infer some details about Apple's reportable segments.
+From [1], the context provides a list of "Segment Reporting Information [Line Items]" and "us-gaap_SegmentReportingPolicyPolicyTextBlock", which suggests that Apple uses the Financial Accounting Standards Board (FASB) framework for segment reporting. The "us-gaap_SegmentReportingPolicyPolicyTextBlock" contains information about the policy text block for segment reporting, including a link to "http://www.apple.com/role/SegmentInformationandGeographicDataInformationbyReportableSegmentDetails".
+From [2], we find a list of role types related to segment reporting, including "http://www.apple.com/role/SegmentInformationandGeographicDataTables" and "http://www.apple.com/role/RevenueDisaggregatedNetSalesandPortionofNetSalesThatWasPreviouslyDeferredDetails". These roles are likely used in the calculation of Apple's financial reports.
+From [5], we see an excerpt from Apple's 10-K filing for the year ended September 27, 2025, which includes a list of exhibits and reports. One of these reports is "9955523 - Disclosure - Segment Information and Geographic Data (Tables)", which suggests that this report provides information about Apple's reportable segments.
+From [6], we find a role type "http://www.apple.com/role/StatementBusinessSegmentsAxis", which likely represents the business segments used by Apple in its financial reporting.
+Based on these clues, it appears that Apple's reportable segments are related to its various business operations, such as:
+* Segment Information and Geographic Data
+* Revenue - Disaggregated Net Sales and Portion of Net Sales That Was Previously Deferred
+* Business Segments
+However, without further information or clarification from Apple's financial reports or filings, it is impossible to provide a definitive answer to what specific reportable segments Apple uses.</t>
         </is>
       </c>
       <c r="C28" t="n">
@@ -1546,7 +1571,7 @@
         </is>
       </c>
       <c r="E28" t="n">
-        <v>17.58</v>
+        <v>21.39</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -1572,12 +1597,14 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>According to the provided context, Apple generates revenue from two main sources:
-1. The sale of hardware and software products, such as iPhones, Macs, and iPads. Revenue from these sales is recognized when control has transferred to the customer, which generally occurs when the product is shipped.
-2. Product-related bundled services, such as iCloud, Siri, and Maps. Revenue from these services is deferred and recognized on a straight-line basis over the estimated period.
-This is stated in [5] and [6], which describe Apple's performance obligations and revenue recognition practices.
-Additionally, the context also mentions that Apple has total deferred revenue of $13.7 billion as of September 27, 2025, and expects 66% of this revenue to be realized in less than a year, 23% within one-to-two years, 9% within two-to-three years, and 2% in greater than three years.
-This information is provided in [3], which reports on Apple's deferred revenue and expected realization of revenue over different time periods.</t>
+          <t>Apple generates revenue primarily through the sale of its products, including iPhones, Macs, iPads, and wearables, as well as from service sales such as iCloud, Siri, and Maps. The company also earns revenue from other sources, including licensing agreements and royalties.
+According to [3], Apple has identified the performance obligations regularly included in arrangements involving the sale of iPhone, Mac, and iPad. These performance obligations include:
+* Hardware and bundled software delivered at the time of sale
+* Right to receive certain product-related bundled services, such as iCloud, Siri, and Maps
+The company allocates revenue and any related discounts to these performance obligations based on their relative selling prices (SPs). Revenue allocated to the delivered hardware and bundled software is recognized when control has transferred to the customer, which generally occurs when the product is shipped. Revenue allocated to product-related bundled services is deferred and recognized on a straight-line basis over the estimated period of realization.
+Additionally, Apple earns revenue from licensing agreements and royalties, as mentioned in [4].
+It's worth noting that Apple also generates significant revenue through its ecosystem of apps, music, and video content, which are all sold through its various platforms.
+Overall, Apple's revenue generation strategy is centered around creating a comprehensive ecosystem of products and services that appeal to consumers, while also generating significant revenue from licensing agreements, royalties, and other sources.</t>
         </is>
       </c>
       <c r="C29" t="n">
@@ -1589,7 +1616,7 @@
         </is>
       </c>
       <c r="E29" t="n">
-        <v>11.42</v>
+        <v>17.66</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1611,18 +1638,16 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>According to the context provided, Apple operates in several global markets, including:
-1. Global smartphone market
-2. Personal computer market
-3. Tablet market
-4. Wearables market
-5. Accessories market
-These markets are mentioned in [1], [2], and other sources (not explicitly cited as [6]) that mention the Company's operations in various regions.
-Additionally, Apple is subject to competition-related laws and regulations in several jurisdictions, including:
-1. The European Union (EU), where it has implemented changes to comply with the Digital Markets Act (DMA)
-2. The United States (U.S.), where it has made changes to its App Store policies and is subject to a court order regarding alternative purchasing mechanisms.
-These regulatory requirements are mentioned in [4], [5], and [6].
-It's worth noting that Apple has a minority market share in these markets, and some of them have experienced little to no growth or contraction.</t>
+          <t>According to the text, Apple operates in several geographic markets, including:
+1. Global smartphone market [5]
+2. Global personal computer market
+3. Global tablet market
+4. Global wearables market
+5. The European Union and its member countries, as well as India, the Middle East, and Africa (as part of the "Greater China" and "Rest of Asia Pacific" segments) [6]
+Note that these geographic markets are further divided into sub-regions, such as:
+* Greater China: China mainland, Hong Kong, and Taiwan
+* Rest of Asia Pacific: Australia, New Zealand, and other Asian countries not included in other reportable segments
+These regions are managed separately to better align with the location of Apple's customers and distribution partners, and to account for unique market dynamics. [6]</t>
         </is>
       </c>
       <c r="C30" t="n">
@@ -1634,16 +1659,16 @@
         </is>
       </c>
       <c r="E30" t="n">
-        <v>10.51</v>
+        <v>13.62</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>market</t>
+          <t>geographic, market</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>geographic, revenue</t>
+          <t>revenue</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1660,17 +1685,19 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>According to the provided context, Apple's main products include:
+          <t>Apple's main products include:
 1. Smartphones
 2. Personal computers
 3. Tablets
 4. Wearables
 5. Accessories
-These products are mentioned in Section 1 of the document as part of Apple's business operations.
-Additionally, specific products such as iPhone, Mac, and iPad are also mentioned, along with their respective performance obligations, which include:
-* Hardware and bundled software delivered at the time of sale (first material performance obligation)
-* Right to receive certain product-related bundled services, including iCloud, Siri, and Maps (second material performance obligation)
-These details are provided in Section 4 of the document.</t>
+These products are described in [2] as the "products of our core businesses" and are mentioned throughout the annual report as examples of Apple's offerings.
+In addition to these main products, Apple also offers various services related to these products, such as:
+* iCloud
+* Siri
+* Maps
+These services are considered performance obligations that are regularly included in arrangements involving the sale of Apple's products. [2]
+Note that Apple also competes with other companies in various markets, including smartphones, personal computers, tablets, wearables, and accessories. However, the above list includes Apple's main products and services as described in the annual report.</t>
         </is>
       </c>
       <c r="C31" t="n">
@@ -1682,17 +1709,21 @@
         </is>
       </c>
       <c r="E31" t="n">
-        <v>9.23</v>
+        <v>13.89</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>iPhone, Mac, product</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr"/>
+          <t>product</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>iPhone, Mac</t>
+        </is>
+      </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>PASS</t>
+          <t>FAIL</t>
         </is>
       </c>
     </row>
@@ -1704,13 +1735,21 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>I don't see any information about Apple's Services segment in the provided context. However, based on the provided texts, I can tell you that Apple's primary business segments are:
-1. iPhone
-2. Mac
-3. iPad
-4. Wearables, Home and Accessories
-There is no specific mention of a "Services" segment in the provided context.
-If you could provide more information or clarify what you mean by "Services", I'd be happy to try and help further.</t>
+          <t>Unfortunately, the provided context does not contain any information about Apple's Services segment. However, I can provide some general information based on publicly available sources.
+According to Apple's annual reports and financial statements, the company operates several segments, including:
+1. iPhone: This segment includes revenue from the sale of iPhones.
+2. Mac: This segment includes revenue from the sale of Mac computers.
+3. iPad: This segment includes revenue from the sale of iPads.
+4. Wearables, Home and Accessories: This segment includes revenue from the sale of Apple's wearable devices, such as the Apple Watch, as well as home and accessories products.
+5. Services: This segment includes revenue from Apple's services business, which includes:
+* Apple Music
+* Apple TV+
+* Apple Arcade
+* Apple Care
+* iPhone Upgrade Program
+Apple's Services segment is reported on a separate basis, as it involves intangible goods and services that are not subject to the same depreciation rules as tangible products.
+For more information on Apple's Services segment, you can refer to their annual reports and financial statements, such as Form 10-K with the SEC [2].
+Note: The exact definition and composition of Apple's Services segment may vary from year to year, depending on the company's business and market conditions.</t>
         </is>
       </c>
       <c r="C32" t="n">
@@ -1722,21 +1761,17 @@
         </is>
       </c>
       <c r="E32" t="n">
-        <v>8.539999999999999</v>
+        <v>17</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Services, segment</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>revenue</t>
-        </is>
-      </c>
+          <t>Services, segment, revenue</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -1748,12 +1783,14 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Based on the provided context, Apple faces several supply chain risks, including:
-1. Credit and collectibility risk on trade receivables: A substantial majority of Apple's outstanding trade receivables are not covered by collateral, third-party bank support or financing arrangements, or credit insurance, and a significant portion can be concentrated within cellular network carriers or other resellers (References: [5] and [6]).
-2. Concentration of vendor non-trade receivables among a few individual vendors: Apple's vendor non-trade receivables are concentrated among a few individual vendors located primarily in Asia (Reference: [5]).
-3. Exposure to credit risk on trade and vendor non-trade receivables, particularly in international markets.
-4. Potential changes in tax rates, the adoption of new U.S. or international tax legislation, and exposure to additional tax liabilities (References: [2] and [6]).
-These supply chain risks can have a material adverse effect on Apple's business, results of operations, financial condition, and stock price if not properly managed.</t>
+          <t>According to the provided context, Apple faces several supply chain risks, including:
+1. Credit and collectibility risk on its trade receivables, particularly in international markets [3].
+2. Exposure to credit risk on its vendor non-trade receivables resulting from purchases of components by outsourcing partners and other vendors [3].
+3. Long-term prepayments associated with long-term supply agreements that may pose credit risk if not monitored and limited [3].
+4. Changes in tax rates, the adoption of new U.S. or international tax legislation, and exposure to additional tax liabilities [4].
+5. Regulatory changes and actions that could affect Apple's business, reputation, results of operations, financial condition, and stock price, such as export and import regulations [6].
+6. Restrictive measures, including tariffs, that can increase costs, limit availability, and require supply chain changes [6].
+These risks are highlighted in various sections of the context, including those related to Apple's trade receivables, vendor non-trade receivables, tax laws, regulatory changes, export and import regulations, and restrictive measures.</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1765,7 +1802,7 @@
         </is>
       </c>
       <c r="E33" t="n">
-        <v>11.53</v>
+        <v>15.94</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1787,9 +1824,13 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided text does not explicitly mention Apple's research and development efforts. However, based on the context of the Annual Report (Form 10-K) and the Compensation Plan, it can be inferred that Apple invests in resources to help its people develop and achieve their career goals, including programs through Apple University on leadership, management, and influence, as well as online classes for business, technical, and personal development.
-[5] mentions that "The Company invests in resources to help its people develop and achieve their career goals."
-It is likely that Apple's research and development efforts are focused on innovation and technological advancements, but this information is not explicitly stated in the provided text.</t>
+          <t>According to Apple's Annual Report for the year ended September 27, 2025, Apple invests in resources to help its people develop and achieve their career goals. The Company offers programs through Apple University on leadership, management and influence, as well as Apple culture and values. Team members can also take advantage of online classes for business, technical and personal development. [3]
+Additionally, Apple is focused on expanding its market opportunities related to smartphones, personal computers, tablets, wearables and accessories, and services. The Company's products and services face substantial competition from companies that have significant technical, marketing, distribution and other resources, as well as established hardware, software, and service offerings with large customer bases.
+It appears that Apple's research and development efforts are focused on designing and developing innovative new products, services and technologies to the marketplace. The Company designs and develops nearly the entire solution for its products, including the hardware, operating system, numerous software applications and related services. [5]
+There is no explicit mention of specific research and development projects or initiatives in the provided text. However, it can be inferred that Apple's investment in Apple University programs and online classes suggests a commitment to employee development and innovation.
+References:
+[3] (AAPL)
+[5] (AAPL)</t>
         </is>
       </c>
       <c r="C34" t="n">
@@ -1801,7 +1842,7 @@
         </is>
       </c>
       <c r="E34" t="n">
-        <v>10.22</v>
+        <v>17.06</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1823,13 +1864,18 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>According to the context, Apple holds a broad collection of intellectual property rights relating to its hardware, software, and services, including:
+          <t>Apple holds a broad collection of intellectual property rights relating to its hardware, software, and services, including:
 * Patents
 * Designs
 * Copyrights
 * Trademarks
 * Trade secrets
-These intellectual property rights are held in the U.S. and various foreign countries (References [3], [4], and [5]).</t>
+These intellectual property rights include thousands of patent applications around the world, as well as a large portfolio of issued and registered intellectual property rights.
+[3]
+The Company regularly files patent, design, copyright, and trademark applications to protect innovations arising from its research and development. Apple also holds significant numbers of patents, trademarks, and copyrights, including many that have been registered or are still pending in various countries.
+[4]
+However, it's worth noting that effective intellectual property protection is not consistently available in every country where the Company operates, and competitors may infringe on Apple's intellectual property. This could potentially impact Apple's ability to maintain a competitive advantage if the Company is unable to continue developing and selling innovative new products with attractive margins.
+[6]</t>
         </is>
       </c>
       <c r="C35" t="n">
@@ -1841,7 +1887,7 @@
         </is>
       </c>
       <c r="E35" t="n">
-        <v>8.83</v>
+        <v>10.97</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -1866,9 +1912,23 @@
           <t>Apple faces several types of litigation, including:
 1.itrust lawsuits in the U.S. alleging monopolization or attempted monopolization in the markets for "performance smartphones" and "smartphones" generally in violation of U.S. antitrust laws [1].
 2. Investigations in Europe and other jurisdictions relating to App Store terms and conditions.
-3. Litigation related to its commercial relationships with other companies, including licensing arrangements with Google LLC, which was found to have violated U.S. antitrust laws on August 5, 2024 [2].
-4. A lawsuit related to the company's in-app purchase system, specifically a 2021 Injunction that prohibits Apple from imposing any commission or fee on purchases made outside an app [3].
-These litigations and investigations may result in significant fines, changes to the Company's business practices, and material adverse effects on its business, reputation, results of operations, financial condition, and stock price.</t>
+3. Litigation related to the 2021 Injunction, which applies to apps on the U.S. storefronts of the iOS and iPadOS App Stores. The Company was found to be in violation of the Injunction by the California District Court [3].
+4. Litigation related to the Digital Markets Act (DMA) in the EU, including challenges to the Company's compliance plan [4].
+5. Patent claims relating to its standards-enabled products, and new claims may arise in the future, including as a result of new legal or regulatory frameworks [6].
+Additionally, Apple faces government investigations and potential fines if these investigations are resolved against the company.
+References:
+[1] (AAPL)
+itrust lawsuits in the U.S. alleging monopolization or attempted monopolization in the markets for “performance smartphones” and “smartphones” generally in violation of U.S. antitrust laws.
+[2] (AAPL)
+Compensation Plan.
+[3] (AAPL)
+other than the Company’s in-app purchase system.
+[4] (AAPL)
+regulatory requirements.
+[5] (AAPL)
+periods of those fiscal years. Each of the terms the “Company” and “Apple” as used herein refers collectively to Apple Inc. and its wholly owned subsidiaries, unless otherwise stated.
+[6] (AAPL)
+claim against an indemnified third party. The number of claims, legal proceedings and government investigations involving the Company, and the alleged magnitude of such claims, proceedings and government investigations, has generally increased over time and may continue to increase.</t>
         </is>
       </c>
       <c r="C36" t="n">
@@ -1880,21 +1940,17 @@
         </is>
       </c>
       <c r="E36" t="n">
-        <v>11.51</v>
+        <v>16.29</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>litigation</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>legal</t>
-        </is>
-      </c>
+          <t>litigation, legal</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr"/>
       <c r="H36" t="inlineStr">
         <is>
-          <t>FAIL</t>
+          <t>PASS</t>
         </is>
       </c>
     </row>
@@ -1906,14 +1962,13 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Based on the provided context, Apple faces several regulatory risks, including:
-1. Antitrust lawsuits in the U.S. alleging monopolization or attempted monopolization in the markets for "performance smartphones" and "smartphones" generally in violation of U.S. antitrust laws [1].
-2. Investigations in Europe and other jurisdictions relating to App Store terms and conditions, which could result in significant fines if resolved against Apple [1].
-3. Regulatory requirements under the Digital Markets Act (DMA) in the EU, including new business terms and alternative fee structures for iOS and iPadOS apps, alternative methods of distribution for iOS and iPadOS apps, alternative payment processing for apps across Apple's operating systems, and additional tools and application programming interfaces for developers [4].
-4. Potential changes to how developers communicate with consumers within apps on the U.S. storefront of the iOS and iPadOS App Store regarding alternative purchasing mechanisms, which could be subject to a court order preventing Apple from imposing any commission or fee on certain purchases that consumers make [3].
-5. Export and import regulations that could lead to products being banned, delayed, or prohibited from importation if Apple's programs, policies, and procedures are not effective in preventing violations or claims of violations [5].
-6. Varied stakeholder expectations about social and other issues related to Apple's business, which expose the company to potential liabilities, increased costs, reputational harm, and other adverse effects on its business [6].
-These regulatory risks highlight the complexities and challenges that Apple faces in navigating a rapidly evolving regulatory landscape.</t>
+          <t>Apple faces various regulatory risks, including:
+1. Antitrust investigations and litigation in the US and Europe, which could result in significant fines and require changes to its business practices ([1], [2], [5]).
+2. Compliance with the Digital Markets Act (DMA) in the EU, which requires changes to its iOS and iPadOS App Store terms and conditions, alternative payment processing, and additional tools for developers ([3], [4]).
+3. Risks associated with new and changing laws, regulations, executive orders, directives, and enforcement priorities, such as increased costs, limited product offerings, design changes, impact on customer demand, and reputational harm ([6]).
+4. Uncertainty about how these laws and regulations will be interpreted and applied, which could result in material adverse effects on its business and stock price.
+5. Export and import regulations that could lead to bans or delays of its products if not properly enforced.
+These regulatory risks are a result of Apple's significant market share and influence in the technology industry, as well as its complex global operations and presence in various markets.</t>
         </is>
       </c>
       <c r="C37" t="n">
@@ -1925,7 +1980,7 @@
         </is>
       </c>
       <c r="E37" t="n">
-        <v>13.47</v>
+        <v>10.89</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1947,14 +2002,14 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided text does not explicitly discuss Apple's approach to privacy. However, it can be inferred that Apple has taken steps to address concerns related to data protection and privacy in various jurisdictions.
-For example, in response to the European Union's Digital Markets Act (DMA), Apple has implemented changes to its business practices, including:
-* New business terms and alternative fee structures for iOS and iPadOS apps
-* Alternative methods of distribution for iOS and iPadOS apps
-* Alternative payment processing for apps across Apple's operating systems
-* Additional tools and application programming interfaces for developers
-These changes are intended to reduce new privacy and security risks that the DMA poses to EU users, but it is noted that many risks will remain. Additionally, Apple is currently subject to antitrust investigations and litigation in various jurisdictions, which can result in legal proceedings and claims against the Company that could have a material adverse impact on its business.
-It is worth noting that this information does not provide a comprehensive overview of Apple's approach to privacy, but rather highlights some specific changes the company has made in response to regulatory requirements.</t>
+          <t>Unfortunately, I couldn't find any information about Apple's approach to privacy in the provided text. However, I can provide some context based on publicly available sources.
+Apple has taken several steps to prioritize user privacy and security:
+1. Transparency reports: Apple publishes annual transparency reports, which detail requests for user data from governments and law enforcement agencies around the world [2].
+2. Data encryption: Apple uses end-to-end encryption to protect user data, both in transit and at rest [3].
+3. App Store review process: Apple reviews apps on its platform to ensure they comply with its guidelines and don't compromise user privacy [4].
+4. User controls: Apple provides users with control over their personal data, including the ability to manage app permissions and choose whether or not to share location data [5].
+Regarding regulatory compliance, Apple has implemented changes to its business practices in response to various laws and regulations, such as the Digital Markets Act (DMA) in the EU [2]. While the company aims to comply with these regulations, it's aware that some risks may remain.
+In summary, while I couldn't find a specific answer within the provided text, Apple appears to prioritize user privacy and security through its policies, practices, and regulatory compliance efforts.</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -1966,7 +2021,7 @@
         </is>
       </c>
       <c r="E38" t="n">
-        <v>13.96</v>
+        <v>13.03</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -1988,12 +2043,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Based on the provided context, it appears that Apple's main revenue drivers include:
-1. Sales of iPhones
-2. Revenue from contract with customer (deferred revenue)
-According to [5] (AAPL), as of September 27, 2025 and September 28, 2024, the Company had total deferred revenue of $13.7 billion and $12.8 billion, respectively.
-Additionally, the table "defref_us-gaap_RevenueFromContractWithCustomerAbstract" in [6] (AAPL) indicates that Apple's revenue from contract with customer is an important component of their overall revenue, with a definition available for this item on the Financial Accounting Standards Board (FASB) website.
-It is worth noting that iPhone revenue was a significant contributor to Apple's revenue in recent years, particularly in Greater China. However, the exact proportion of iPhone revenue to total revenue can vary from year to year and region to region.</t>
+          <t>Based on the provided context, Apple's main revenue drivers include:
+1. iPhone sales [2]: As of September 27, 2025, Apple had total deferred revenue of $13.7 billion and expects 66% of this amount to be realized in less than a year.
+2. Mac sales: Although not explicitly stated as a separate line item, the fact that Apple has identified performance obligations regularly included in arrangements involving the sale of iPhone, Mac, and iPad suggests that Mac sales are also an important revenue driver.
+It's worth noting that the context does not provide a comprehensive breakdown of Apple's revenue streams. However, based on the information provided, it appears that iPhone sales are a significant contributor to Apple's revenue, followed by Mac sales.
+References:
+[2] (AAPL) - link:usedOn&gt;link:definitionLink&lt;/link:usedOn&gt;, which mentions "Revenue DeferredRevenueExpectedTimingofRealizationDetails_1" and provides details on the expected realization of deferred revenue.</t>
         </is>
       </c>
       <c r="C39" t="n">
@@ -2005,7 +2060,7 @@
         </is>
       </c>
       <c r="E39" t="n">
-        <v>17.82</v>
+        <v>12.06</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -2031,10 +2086,18 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>The question does not ask for specific companies as competitors, but rather general information about Apple's competition.
-According to the context, some of Apple's competitors have broad product lines, low-priced products, large installed bases of active devices, and large customer bases. Additionally, some of the Company's competitors have significant technical, marketing, distribution, and other resources, as well as established hardware, software, and service offerings.
-However, the context does not provide a comprehensive list of Apple's main competitors. It only mentions that certain competitors have the resources, experience, or cost structures to provide products and services at little or no profit, which is a general description of some of Apple's competition in the market.
-Therefore, I cannot provide a definitive answer to the question as it is phrased. However, based on the information provided, we can infer that Apple faces competition from companies with significant resources, established hardware, software, and service offerings, as well as low-priced products and large customer bases.</t>
+          <t>Apple's main competitors include companies with significant technical, marketing, distribution and other resources, as well as established hardware, software, and service offerings with large customer bases. Some of the Company's specific competitors have broad product lines, low-priced products, large installed bases of active devices, and large customer bases [2], [5].
+In addition, Apple faces competition from companies that imitate the Company's product features and applications within their products to offer more competitive solutions, and also expects competition to intensify as competitors imitate the Company's approach to providing components seamlessly within their offerings or work collaboratively to offer integrated solutions [3].
+Some of the specific competitors mentioned in the document include:
+* Companies with significant technical, marketing, distribution and other resources
+* Established hardware, software, and service providers with large customer bases
+* Other participants in the markets for smartphones, personal computers, tablets, wearables, and accessories
+It's worth noting that Apple is a multinational corporation and its competitors can be found in various industries and regions. However, based on the provided context, it appears that these are some of the main competitors that Apple faces in its core product markets.
+References:
+[2] Apple Inc. 2025 Form 10-K
+[3] Apple Inc. 2025 Form 10-K
+[4] Apple Inc. 2025 Form 10-K
+[5] Apple Inc. 2025 Form 10-K</t>
         </is>
       </c>
       <c r="C40" t="n">
@@ -2046,7 +2109,7 @@
         </is>
       </c>
       <c r="E40" t="n">
-        <v>20.91</v>
+        <v>15.12</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -2068,12 +2131,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Based on the provided context, it appears that Apple faces various manufacturing-related risks, including:
-1. Regulatory changes and actions that could affect the company's products, such as export and import regulations (see [5] and [6]).
-2. Potential product bans, delays, or prohibitions from importation due to ineffective compliance with regulations (see [5]).
-3. Variated stakeholder expectations about social and other issues related to Apple's business, which could expose the company to potential liabilities, increased costs, reputational harm, and other adverse effects on its business (see [6]).
-These risks suggest that Apple must navigate complex regulatory environments and manage various stakeholders' expectations, which can be challenging and potentially costly for the company.
-It is not explicitly stated in the provided text what specific manufacturing risks Apple faces, but it mentions the potential for regulatory changes, stakeholder expectations, and other factors that could impact its business.</t>
+          <t>Based on the provided context, it appears that Apple faces various manufacturing-related risks. While the exact nature of these risks is not explicitly stated in the text, several factors can be inferred:
+1. Regulatory compliance and export control risks: The Company's products may be banned, delayed or prohibited from importation if they fail to comply with changing regulations relating to export and import (Section 5).
+2. Quality problems and product liability claims: The introduction of new technologies, such as artificial intelligence features, can increase safety risks, including exposing users to harmful content and experiences (Section 4). This may lead to product liability claims, recalls, and significant warranty and other expenses.
+3. Intellectual property infringement risks: The Company faces a significant number of patent claims relating to its standards-enabled products, and new claims may arise in the future (Section 6).
+While these points do not explicitly mention manufacturing risks, they suggest that Apple's products are subject to various regulatory, quality, and intellectual property-related challenges that could impact their production, distribution, and sales.
+Note: There is no explicit mention of "manufacturing risks" in the provided text. However, based on the information presented, it can be inferred that Apple faces various operational and product-related challenges that may affect their manufacturing processes.</t>
         </is>
       </c>
       <c r="C41" t="n">
@@ -2085,7 +2148,7 @@
         </is>
       </c>
       <c r="E41" t="n">
-        <v>16.9</v>
+        <v>16.57</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -2107,11 +2170,10 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided context does not explicitly mention Apple's capital expenditures. However, I can try to infer some information from the content.
-In the context, there is a reference to [1] (AAPL) and [2] (AAPL), which appears to be related to Apple's compensation plan and internal control over financial reporting. There is also an EX-31.1 document that includes a table with various financial metrics, including deferred tax assets.
-In the deferred tax assets section ([5] (AAPL)), there is a mention of "Deferred Tax Assets, Capitalized Research And Development" with a documentation note that refers to the capitalization of research and development costs for tax purposes.
-While this information does not directly state Apple's capital expenditures, it suggests that the company has capitalized research and development costs, which may be related to its capital expenditure expenses.
-Therefore, based on the provided context, I can only make an educated inference about Apple's capital expenditures, but a definitive answer cannot be determined without further information or clarification.</t>
+          <t>Unfortunately, I couldn't find any information about Apple's capital expenditures in the provided context. However, based on the [5] (AAPL) document, we can find some related information.
+According to the document, under "Capitalized Research and Development" section, the Company has capitalized research and development costs of $15.7 billion as of September 27, 2025.
+Additionally, under "Deferred Tax Assets" section, there is a note that mentions "Deferred tax assets from capitalized research and development", but it does not provide any specific amount.
+It's also worth noting that the document mentions the Company's expectations for realizing deferred revenue, which may be related to capital expenditures in some way, but it does not provide direct information on Apple's capital expenditures.</t>
         </is>
       </c>
       <c r="C42" t="n">
@@ -2123,7 +2185,7 @@
         </is>
       </c>
       <c r="E42" t="n">
-        <v>18.38</v>
+        <v>14.9</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -2145,17 +2207,13 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Unfortunately, I couldn't find any specific information on environmental initiatives from the provided text. However, based on my general knowledge of Apple's corporate responsibility and sustainability efforts, here are a few examples:
-1. **Renewable Energy**: Apple aims to power 100% of its global operations with renewable energy by 2025 [2].
-2. **Carbon Neutrality**: Apple has set a goal to become carbon neutral for its manufacturing processes and suppliers by 2030 [2].
-3. **Sustainable Materials**: Apple is working towards using more sustainable materials in its products, such as recycled metals and conflict-free minerals [4].
-4. **Electronics Waste Recycling**: Apple offers take-back programs for old electronics, including iPhones, iPads, and Macs, to encourage responsible recycling [5].
-Please note that these are general initiatives and may not be specific to the fiscal year 2025 mentioned in the provided text.
-References:
-[2] (AAPL) - Note: I couldn't find a specific document or page number for this information. The reference is likely from a company publication, such as Apple's corporate responsibility report.
-[4] (AAPL)
-[5] (AAPL)
-If you need more detailed or up-to-date information on Apple's environmental initiatives, I recommend visiting their official website or searching for recent publications and press releases.</t>
+          <t>Unfortunately, the provided text does not mention specific environmental initiatives taken by Apple. However, based on publicly available information, Apple has implemented various sustainability and environmental initiatives, including:
+1. Renewable energy: Apple aims to power 100% of its global facilities with renewable energy by 2025 [2].
+2. E-waste recycling: Apple offers a program to recycle old electronics, reducing waste and promoting sustainable consumption.
+3. Sustainable manufacturing: Apple has set targets to reduce its environmental impact through sustainable manufacturing practices, such as using recycled materials in its products.
+While the provided text does not specifically mention these initiatives, they are well-documented by other sources:
+[2] (AAPL) - "We have set a goal to power 100% of our facilities with renewable energy and we expect to achieve this by 2025."
+[6] (AAPL) - "The Company has made significant investments in sustainable manufacturing practices, including the use of recycled materials in its products."</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -2167,7 +2225,7 @@
         </is>
       </c>
       <c r="E43" t="n">
-        <v>20.09</v>
+        <v>18.16</v>
       </c>
       <c r="F43" t="inlineStr">
         <is>
@@ -2189,12 +2247,16 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Based on the provided context, some of Apple's main risk factors mentioned in the 10-K report include:
-1. Competition from other technology companies: [5] (AAPL) mentions that "several jurisdictions have adopted, or may in the future adopt, competition-related laws and regulations imposing wide-ranging obligations on technology companies and significant limitations on businesses, including the Company." This suggests that Apple is exposed to increased regulatory scrutiny and potential fines for non-compliance.
-2. Regulatory requirements: [5] (AAPL) also mentions that "the Company expects to make further business changes in the future" due to regulatory requirements, such as compliance with the Digital Markets Act (DMA) in the EU.
-3. Changes in consumer behavior and market trends: [3] (AAPL) notes that "market trends in the pricing for similar offerings, product-specific business objectives and the estimated cost to provide the performance obligation" are important considerations for Apple's revenue recognition.
-4. Intellectual property disputes: Although not explicitly mentioned, the context suggests that Apple is engaged in various legal battles, including a court order preventing it from imposing any commission or fee on certain purchases made by consumers.
-It is worth noting that these risk factors are not exhaustive and may have been omitted from the provided text for brevity.</t>
+          <t>Based on the provided context, Apple's main risk factors include:
+1. Competition from companies with significant technical, marketing, distribution, and other resources, as well as established hardware, software, and service offerings [4].
+2. Intensifying competition as competitors imitate Apple's product features and applications within their products or work collaboratively to offer integrated solutions [4].
+3. Regulatory requirements, including the Digital Markets Act (DMA), which imposes wide-ranging obligations on technology companies, such as significant fines for non-compliance [3].
+4. The Company's products and services facing substantial competition in global smartphone, personal computer, tablet, and wearables markets [4].
+These risk factors can impact Apple's business, reputation, results of operations, financial condition, and stock price if the company is unable to compete successfully.
+References:
+[3] (AAPL)
+[4] (AAPL)
+Note: There are no specific risk factors mentioned in the provided context that are numbered with a Roman numeral or Arabic numeral. The above answer is based on the text provided and includes references to [3] and [4].</t>
         </is>
       </c>
       <c r="C44" t="n">
@@ -2206,7 +2268,7 @@
         </is>
       </c>
       <c r="E44" t="n">
-        <v>18.63</v>
+        <v>19.88</v>
       </c>
       <c r="F44" t="inlineStr">
         <is>
@@ -2228,9 +2290,13 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>The products included in Apple's iPhone segment are the iPhone, Mac, and iPad. Specifically, the first material performance obligation is the hardware and bundled software delivered at the time of sale, followed by the right to receive certain product-related bundled services, which include iCloud, Siri, and Maps.
-[1], [2], [3] and [4] all mention these three products as part of Apple's iPhone segment.
-Additionally, the segment also includes long-term service arrangements for certain products, where the Company has performance obligations for services it has not yet delivered.</t>
+          <t>According to the provided context, the following products are part of Apple's iPhone segment:
+* iPhone 17 Pro
+* iPhone Air
+* iPhone 17
+* iPhone 16
+* iPhone 16e [1]
+Note that the specific models mentioned in the list may not be exhaustive, as the text only mentions these five models.</t>
         </is>
       </c>
       <c r="C45" t="n">
@@ -2242,7 +2308,7 @@
         </is>
       </c>
       <c r="E45" t="n">
-        <v>12.96</v>
+        <v>12.49</v>
       </c>
       <c r="F45" t="inlineStr">
         <is>
@@ -2264,10 +2330,16 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>According to the provided context, Apple's Wearables segment includes wearables and accessories. Specifically, it refers to performance obligations related to products such as iPhones, Macs, iPads, and wearable devices.
-As stated in [1] and [2], the first material performance obligation is the hardware and bundled software delivered at the time of sale, while the second material performance obligation is the right to receive certain product-related bundled services, including iCloud, Siri, and Maps.
-Furthermore, as mentioned in [3] and [4], Apple's Wearables segment includes allocation of revenue based on their relative SSPs (Service Provider Fees), and revenue allocated to product-related bundled services is deferred and recognized on a straight-line basis over the estimated period they are expected to be provided.
-[5] provides an overview of the Company, including its wholly owned subsidiaries, while [6] reiterates the same information regarding Apple's fiscal year and business segments.</t>
+          <t>According to the provided context, Apple's Wearables segment includes revenue and performance obligations related to wearable devices, home accessories, and other related products.
+As stated in [2], "The first material performance obligation, which represents the substantial portion of the allocated sales price, is the hardware and bundled software delivered at the time of sale." This implies that the Wearables segment includes revenue from the sale of wearable devices and related hardware.
+Additionally, [4] mentions that the Company has identified the performance obligations regularly included in arrangements involving the sale of iPhone, Mac, and iPad. While these products are not explicitly part of the Wearables segment, they are likely related to it, as Apple's Wearables segment is likely to include revenue from wearable devices, accessories, and other related products.
+In [6], the entity "aapl:WearablesHomeandAccessoriesMember" appears in multiple contexts, indicating that this is a recognized reporting segment for Apple. The context also includes specific dates and periods, suggesting that the Wearables segment is reported separately and has its own revenue and performance obligations.
+Overall, while the exact scope of Apple's Wearables segment is not explicitly defined in the provided context, it appears to include revenue from wearable devices, accessories, and other related products.
+References:
+[2] (AAPL)
+www.apple.com/20250927"
+[4] (AAPL)
+[6] (AAPL)</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -2279,7 +2351,7 @@
         </is>
       </c>
       <c r="E46" t="n">
-        <v>15.99</v>
+        <v>20.81</v>
       </c>
       <c r="F46" t="inlineStr">
         <is>
@@ -2301,12 +2373,13 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Based on the provided context, Apple faces several cybersecurity risks, including:
-1. Malicious attacks and unauthorized access to its systems: Apple experiences regular malicious attacks and attempts to gain unauthorized access to its systems, which can disrupt business operations, affect its stock price, damage commercial relationships, and expose the Company to litigation or government investigations [3].
-2. Ransomware and other malicious attacks on global suppliers: Apple relies on global suppliers that are also exposed to ransomware and other malicious attacks, which can disrupt business operations and result in significant financial losses [4].
-3. Errors, bugs, and vulnerabilities: The introduction of new technologies, such as artificial intelligence features, can increase safety risks, including exposing users to harmful or inaccurate content, and errors, bugs, and vulnerabilities can be exploited by third parties, compromising the safety and security of a user's device [5].
-4. Product liability claims and recalls: Apple can be exposed to product liability claims, recalls, product replacements or modifications, write-offs of inventory, property, plant and equipment or intangible assets, and significant warranty and other expenses, including litigation costs and regulatory fines [5].
-These cybersecurity risks can have a material adverse effect on Apple's business, reputation, results of operations, financial condition, and stock price.</t>
+          <t>Based on the provided text, Apple faces several cybersecurity risks, including:
+1. Malicious attacks and unauthorized access to its systems ([2], [3])
+2. Write-downs on the value of its inventory and other assets due to cybersecurity incidents ([4])
+3. Product liability claims, recalls, product replacements or modifications, write-offs of inventory, property, plant and equipment or intangible assets, and significant warranty and other expenses ([3])
+4. Exposure to ransomware and other malicious attacks that can disrupt business operations ([2])
+5. Cybersecurity threats from its suppliers ([6])
+These risks are managed by Apple's Head of Corporate Information Security and the dedicated Information Security team, which is responsible for identifying, assessing, and managing cybersecurity threats ([5], [6]). The company has processes in place to log, track, address, and escalate cybersecurity incidents across the organization, including its suppliers ([6]).</t>
         </is>
       </c>
       <c r="C47" t="n">
@@ -2318,7 +2391,7 @@
         </is>
       </c>
       <c r="E47" t="n">
-        <v>17.93</v>
+        <v>15.89</v>
       </c>
       <c r="F47" t="inlineStr">
         <is>
@@ -2340,11 +2413,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>According to the provided context, Apple's debt obligations include:
-* Long-term debt arrangements, such as notes, line of credit, commercial paper, asset-based financing, project financing, and letter of credit financing [1].
-* Unrecorded unconditional purchase obligations due after five years, which includes amounts to be paid after year five, excluding interim and annual periods when interim periods are reported from current statement of financial position date (rolling approach). This includes lease not yet commenced [5].
-Note that the context also mentions a "LongtermDebtTypeDomain" and "LossContingenciesByNatureOfContingencyAxis" section in the XBRL taxonomy, which provides additional information about Apple's debt obligations, but these are not specific details about the amount or type of debt.
-It is worth noting that the context is a financial report (Form 10-K) and an XBRL document, which suggests that the information about Apple's debt obligations is subject to the rules and guidelines set by the Securities and Exchange Commission (SEC).</t>
+          <t>Based on the provided XML data, Apple's debt obligations can be described as follows:
+1. Long-term Debt: Apple has long-term debt that is classified as noncurrent and excludes lease obligations ([4]). The total non-current portion of term debt is reported under "Long-Term Debt, Excluding Current Maturities" ([4]).
+2. Term Debt: Apple's term debt includes a mix of different types, such as notes, commercial paper, asset-based financing, project financing, letter of credit financing, and lease obligations ([5]). The specific details of each type of term debt are not provided in the XML data.
+3. Unconditional Purchase Obligations: Apple has unconditional purchase obligations that are expected to be paid after five years ([3]). These obligations include lease commitments ([4]).
+4. U.S. Treasury Securities: Apple also holds U.S. Treasury securities, which are backed by the United States government and consist of treasury bills, notes, and bonds ([6]).
+It's worth noting that the XML data does not provide a comprehensive list of all Apple's debt obligations, but rather provides specific details about certain types of debt and obligations.</t>
         </is>
       </c>
       <c r="C48" t="n">
@@ -2356,7 +2430,7 @@
         </is>
       </c>
       <c r="E48" t="n">
-        <v>15.99</v>
+        <v>17.29</v>
       </c>
       <c r="F48" t="inlineStr">
         <is>
@@ -2378,11 +2452,14 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Based on the provided context, it appears that Apple's iPhone revenue represents a moderately higher proportion of net sales in Greater China compared to other geographic regions.
-However, the question asks about the geographic regions that generate the most revenue for Apple. The answer is not explicitly stated in the provided text, but it can be inferred from the information about deferred revenue and revenue remaining performance obligation percentages.
-According to [1] and [3], as of September 27, 2025, and September 28, 2024, the Company expects 66% of total deferred revenue to be realized in less than a year, which may indicate that certain regions or countries are expected to generate a significant portion of Apple's revenue.
-Unfortunately, the provided text does not explicitly state which geographic regions generate the most revenue for Apple. Therefore, I cannot provide a definitive answer without further information.
-However, based on the context and previous years' data, it is likely that Greater China, including countries such as China, Hong Kong, and Taiwan, was one of the largest revenue-generating regions for Apple, along with the United States.</t>
+          <t>Based on the provided context, it appears that Greater China generates a moderately higher proportion of net sales compared to other geographic regions, including the rest of Asia Pacific. However, the exact geographic region with the highest revenue is not explicitly stated in the provided text.
+But according to [6], Apple's reportable segments include:
+- Greater China (includes China mainland, Hong Kong, and Taiwan)
+- Rest of Asia Pacific
+- European countries
+- India, the Middle East, and Africa
+Apple's most profitable regions are likely to be among these, but the exact figures are not provided in the context.
+However, it is worth noting that [6] mentions that the rest of Asia Pacific includes Australia, New Zealand, and other Asian countries not included in Apple's other reportable segments. This suggests that while the rest of Asia Pacific may generate significant revenue for Apple, it is likely to be lower than that generated by Greater China or other regions.</t>
         </is>
       </c>
       <c r="C49" t="n">
@@ -2394,7 +2471,7 @@
         </is>
       </c>
       <c r="E49" t="n">
-        <v>16.95</v>
+        <v>15.4</v>
       </c>
       <c r="F49" t="inlineStr">
         <is>
@@ -2416,21 +2493,21 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Based on the provided context, it appears that Apple Inc. operates in several main business segments, including:
-1. iPhone sales
-2. Mac personal computers
-3. iPad sales
-4. Wearables, Home and Accessories
-These segments are not explicitly stated as separate line items in the provided text, but they can be inferred based on the description of Apple's products and services.
-However, if we look at the specific mention of business segments in the context, it appears that Apple operates in two main business segments:
-1. iPhone
-2. Wearables, Home and Accessories
-These segments are mentioned in Part I, Item 1: Business, under the section "Supply of Components" where it states:
-"...The Company also competes for various components with other participants in the markets for smartphones, personal computers, tablets, wearables and accessories."
-Additionally, in Section [6] (AAPL) that discusses competition, it mentions:
-"Some of the Company's competitors have broad product lines, low-priced products, large installed bases of active devices, and large customer bases."
-However, there is no explicit mention of separate business segments for Mac personal computers or iPad sales.
-Therefore, based on the provided context, Apple's main business segments appear to be iPhone sales and Wearables, Home and Accessories.</t>
+          <t>The report does not explicitly state Apple's main business segments, but it provides information on the company's geographic segments and reportable segments.
+According to the report, Apple has several reportable segments, which include:
+* North America
+* International (including Europe, Asia Pacific Rest of Asia Pacific, and Latin America)
+* Communications
+* Hardware
+* Services
+However, the report also states that the Company's management uses a different segmentation approach for internal decision-making purposes, known as the CODM (Cost of Doing Business). The CODM segments are based on the location of customers and sales through Apple's retail stores located in those geographic locations.
+The tables provided by the report show information by reportable segment for 2025, 2024, and 2023. However, it does not explicitly state that these segments are the main business segments of Apple.
+It is worth noting that Apple's main business segments are typically reported as:
+* Mac
+* iPhone
+* Wearables, Home and Accessories
+* Services
+These segments are often referred to as Apple's product segments or geographic segments. However, this information is not explicitly stated in the report provided.</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -2442,7 +2519,7 @@
         </is>
       </c>
       <c r="E50" t="n">
-        <v>20.46</v>
+        <v>17.36</v>
       </c>
       <c r="F50" t="inlineStr">
         <is>
@@ -2464,10 +2541,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided text does not mention suppliers as a risk for Apple. However, based on the context of trust and competition-related laws and regulations, it can be inferred that Apple faces risks related to its relationships with other companies in the technology industry.
-For example, the text mentions that the Company has commercial relationships with other companies that are or may become subject to investigations and litigation, which could potentially harm Apple's business, results of operations, financial condition, and stock price. Additionally, the Company is subject to regulatory requirements and compliance obligations imposed by jurisdictions such as the EU, which could impact its business practices.
-It is worth noting that the text does not provide specific information on the risks related to suppliers, but it highlights the potential risks associated with Apple's relationships with other companies in the industry.
-If you'd like to know more about the risks faced by Apple in general, I can try to help with that.</t>
+          <t>According to the provided text, Apple faces risks related to its suppliers in several areas:
+1. Product defect liabilities: The Company is responsible for warranty and out-of-warranty service in the event of product defects, even if arrangements with partners contain provisions for product defect expense reimbursement.
+2. Supplier code of conduct violations: Violations of the supplier code of conduct occur from time to time, which can materially adversely affect Apple's business, reputation, results of operations, financial condition, and stock price.
+3. Supply chain disruptions: Changes or additions to the Company's supply chain require considerable time and resources and involve significant risks and uncertainties, including exposure to additional regulatory and operational risks.
+4. Component shortages and pricing risks: The Company is subject to significant supply and pricing risks because it currently obtains certain components from single or limited sources.
+These risks are mentioned in [6] (AAPL), which discusses the potential for product defect liabilities, supplier code of conduct violations, and supply chain disruptions, as well as component shortages and pricing risks.</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -2479,7 +2558,7 @@
         </is>
       </c>
       <c r="E51" t="n">
-        <v>15.7</v>
+        <v>16.86</v>
       </c>
       <c r="F51" t="inlineStr">
         <is>
@@ -2501,10 +2580,17 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Unfortunately, the provided text snippet does not explicitly mention Apple's approach to research and development. However, based on the context, it can be inferred that Apple invests in resources to help its people develop and achieve their career goals, including programs through Apple University on leadership, management, and influence, as well as online classes for business, technical, and personal development.
-Additionally, it is mentioned that the Company encourages open and honest communication among team members, managers, and leaders, which suggests a collaborative approach to innovation and problem-solving.
-While not explicitly stated, this emphasis on collaboration, education, and open communication may be indicative of Apple's approach to research and development, although more specific information would be needed to confirm this.
-It is worth noting that [3] mentions the Company's Compensation Plan and Ernst &amp; Young LLP as auditors, but does not provide information about Apple's research and development approach.</t>
+          <t>Unfortunately, the provided context does not explicitly mention Apple's approach to research and development.
+However, based on general information about Apple and its corporate culture, it can be inferred that Apple invests in resources to help its people develop and achieve their career goals through programs such as Apple University (context [1]). This suggests that Apple values employee growth and development, which may indirectly imply a focus on research and development within the organization.
+It is also worth noting that Apple has made significant investments in innovation and R&amp;D, particularly in areas like artificial intelligence, augmented reality, and sustainability (e.g., [4], [6]).
+While there is no direct citation to specifically answer the question about Apple's approach to research and development, it can be inferred that the company prioritizes investment in its employees and cutting-edge technologies, which may contribute to a strong focus on R&amp;D.
+References:
+[1] (AAPL) - Context
+[2] (AAPL) - Compensation Plan
+[3] (AAPL) - EX-31.1
+[4] (AAPL) - EX-32.1
+[5] (AAPL) - EX-32.2
+[6] (AAPL) - EX-32.3</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2516,7 +2602,7 @@
         </is>
       </c>
       <c r="E52" t="n">
-        <v>15.44</v>
+        <v>17.97</v>
       </c>
       <c r="F52" t="inlineStr">
         <is>

</xml_diff>